<commit_message>
Fix bug and add modeling lexicon
</commit_message>
<xml_diff>
--- a/delete.xlsx
+++ b/delete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baha Tegar\Desktop\aspect-based-sentiment-analysis-demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112E5FF7-BD57-476C-BBC6-59CBE35635F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC43C4B3-6BD7-43BF-AFB9-1F6CC5010B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="313">
   <si>
     <t>reviewer_id</t>
   </si>
@@ -37,7 +37,7 @@
     <t>aspect</t>
   </si>
   <si>
-    <t>abilities</t>
+    <t>ability</t>
   </si>
   <si>
     <t>3 months ago</t>
@@ -50,7 +50,7 @@
     <t>{0: [], 1: ['normal transaction'], 2: ['substance'], 3: []}</t>
   </si>
   <si>
-    <t>{0: [], 1: ['transaction = normal'], 2: ['substance = milky', 'substance = clear'], 3: ['* = come']}</t>
+    <t>{0: [], 1: [('transaction', 'normal')], 2: [('substance', 'milky'), ('substance', 'clear')], 3: []}</t>
   </si>
   <si>
     <t>5 days ago</t>
@@ -59,10 +59,10 @@
     <t>It'd McDonalds. It is what it is as far as the food and atmosphere go. The staff here does make a difference. They are all friendly, accommodating and always smiling. Makes for a more pleasant experience than many other fast food places.</t>
   </si>
   <si>
-    <t>{0: [], 1: ['food', 'atmosphere'], 2: ['staff here', 'difference'], 3: [], 4: ['experience', 'food places']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['food = go', 'atmosphere = go'], 2: ['staff = make'], 3: [], 4: ['experience = pleasant', 'food = fast', 'places = many', 'places = other']}</t>
+    <t>{0: [], 1: ['food', 'atmosphere'], 2: ['staff here'], 3: [], 4: ['experience', 'food places']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('food', 'go'), ('atmosphere', 'go')], 2: [('staff', 'make')], 3: [], 4: [('experience', 'pleasant'), ('food', 'fast'), ('place', 'many'), ('place', 'other')]}</t>
   </si>
   <si>
     <t>Made a mobile order got to the speaker and checked it in.
@@ -72,22 +72,22 @@
 Went there in person the next day  and the manager told me she wasnÃÂ¯ÃÂ¿</t>
   </si>
   <si>
-    <t>{0: ['mobile order'], 1: ['Line'], 2: ['refund'], 3: ['money'], 4: ['next day', 'manager']}</t>
-  </si>
-  <si>
-    <t>{0: ['order = mobile', 'order = get'], 1: ['Line = move'], 2: [], 3: [], 4: ['day = next', 'manager = tell']}</t>
+    <t>{0: ['mobile order'], 1: ['line'], 2: [], 3: [], 4: ['next day', 'manager']}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'mobile'), ('order', 'get')], 1: [('line', 'move'), ('line', 'have')], 2: [], 3: [('line', 'call'), ('line', 'say'), ('line', 'get')], 4: [('day', 'next'), ('manager', 'tell'), ('manager', 'wasn')]}</t>
   </si>
   <si>
     <t>a month ago</t>
   </si>
   <si>
-    <t>My mc. Crispy chicken sandwich was ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ customer service was quick and p</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['Crispy chicken sandwich', 'customer service']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['sandwich = crispy', 'service = quick']}</t>
+    <t>My mc. Crispy chicken sandwich was ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿Ã</t>
+  </si>
+  <si>
+    <t>{0: [], 1: ['crispy chicken sandwich', 'customer service']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('sandwich', 'crispy')]}</t>
   </si>
   <si>
     <t>2 months ago</t>
@@ -96,10 +96,10 @@
     <t>I repeat my order 3 times in the drive thru, and she still manage to mess it up , it was suppose to be a large meal double filet of fish with large fries , no cheese . It was all wrong , they either need to pay close attention to the order being made , understand English or they need not to work at a drive thru</t>
   </si>
   <si>
-    <t>{0: ['order', 'large meal double filet', 'large fries'], 1: ['close attention', 'drive thru']}</t>
-  </si>
-  <si>
-    <t>{0: ['meal = large', 'filet = double', 'fries = large'], 1: ['attention = close']}</t>
+    <t>{0: ['order', 'large meal double filet', 'large fries'], 1: ['drive thru']}</t>
+  </si>
+  <si>
+    <t>{0: [('filet', 'double'), ('fry', 'large')], 1: []}</t>
   </si>
   <si>
     <t>3 weeks ago</t>
@@ -108,19 +108,19 @@
     <t>I work for door dash and they locked us all out to wait in a long line for no reason at 10. I tried to beg them to open it because I'm door dash and they refused.  Covid is over get a new job</t>
   </si>
   <si>
-    <t>{0: ['door dash', 'long line'], 1: ['door dash'], 2: ['new job']}</t>
-  </si>
-  <si>
-    <t>{0: ['line = long'], 1: ['dash = door'], 2: ['job = new']}</t>
+    <t>{0: ['door dash', 'long line'], 1: ['door dash'], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('line', 'long')], 1: [('dash', 'door')], 2: []}</t>
   </si>
   <si>
     <t>If I  could give this location a zero on customer service, I  would. Pulled into drive through at 8:07 and placed a simple order. I order a regular hamburg and cookies. Once I paid and pulled up to the window to pick up, I  was told to pull up to the #1 space. I sat there and sat there and.........25 minutes later, no order. I  went in and no one was at the counter. I yelled "hello" three times. A young lady came up asking who was handling the front counter. A young girl appeared. To make this complaint shorter, I  showed my receipt and another 5 minutes later I got my order. There was another order with a drink sitting on the counter that never got to the person who ordered it. After getting home, I  had no regular hamburg but had cookies. Everyone, don't even bother going to this location again. It's a horrible experience every time as you can see by other reviews.</t>
   </si>
   <si>
-    <t>{0: ['customer service'], 1: ['simple order'], 2: ['regular hamburg', 'cookies'], 3: [], 4: [], 5: ['one'], 6: [], 7: ['young lady', 'front counter'], 8: ['young girl'], 9: ['complaint', 'receipt', 'order'], 10: [], 11: ['regular hamburg', 'cookies'], 12: [], 13: ['experience', 'other reviews']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['order = simple'], 2: ['into = order', 'hamburg = regular', 'cookies = regular'], 3: [], 4: [], 5: [], 6: [], 7: ['lady = young', 'lady = come', 'counter = front'], 8: ['girl = young', 'girl = appear'], 9: [], 10: [], 11: ['hamburg = regular'], 12: [], 13: ['experience = horrible', 'reviews = other']}</t>
+    <t>{0: ['customer service'], 1: ['simple order'], 2: ['regular hamburg'], 3: [], 4: [], 5: ['one'], 6: [], 7: ['front counter'], 8: [], 9: ['order'], 10: [], 11: ['regular hamburg'], 12: [], 13: ['experience']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('order', 'simple')], 2: [('hamburg', 'regular')], 3: [], 4: [], 5: [], 6: [('one', 'yell')], 7: [('counter', 'front')], 8: [], 9: [], 10: [], 11: [('hamburg', 'regular')], 12: [], 13: [('experience', 'horrible')]}</t>
   </si>
   <si>
     <t>a year ago</t>
@@ -129,37 +129,37 @@
     <t>Came in and ordered a Large coffee w/no ice. They handed me a cup that was less than half way full. I asked the employee, Flor, if they could give me a Large coffee w/no ice and she said no. I was willing to pay more to get a full cup of coffee. I always get a large sweet tea w/no ice and itÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½</t>
   </si>
   <si>
-    <t>{0: ['Large coffee', 'ice'], 1: ['cup', 'half way'], 2: ['employee', 'Large coffee', 'ice'], 3: ['full cup'], 4: ['tea', 'ice'], 5: []}</t>
-  </si>
-  <si>
-    <t>{0: ['w = large'], 1: ['in = full', 'half = less'], 2: ['w = large'], 3: ['cup = full'], 4: ['ice = large', 'ice = sweet'], 5: []}</t>
+    <t>{0: ['large coffee', 'ice'], 1: ['cup'], 2: ['employee', 'large coffee', 'ice'], 3: ['full cup'], 4: ['ice'], 5: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: [('cup', 'full')], 4: [('ice', 'large'), ('ice', 'sweet')], 5: []}</t>
   </si>
   <si>
     <t>Went thru drive thru. Ordered. Getting home noticed my 10 piece nuggets where missing. Tried calling the restaurant and nothing. The lady gave me a hard time about extra sauce. Very unhappy .....</t>
   </si>
   <si>
-    <t>{0: [], 1: [], 2: ['piece nuggets'], 3: ['restaurant'], 4: ['lady', 'time', 'extra sauce'], 5: []}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: [], 2: [], 3: [], 4: ['lady = give', 'time = hard', 'sauce = extra'], 5: []}</t>
+    <t>{0: [], 1: [], 2: ['piece nuggets'], 3: [], 4: ['time'], 5: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [('time', 'hard')], 5: []}</t>
   </si>
   <si>
     <t>I'm not really a huge fan of fast food, but I have 2 teenage daughter's who enjoy McDs. The staff here is always friendly and ALWAYS get their orders correct. By far one of the best McDs I have ever been to. I always enjoy and appreciate quality service from quality people... and you'll definitely find it here. At least from the evening crew. Haven't been here during the day. My girls joke that I go here so often to get them food, that the staff is going to end up knowing me and having their order ready to go. Lmao Great people and excellent service. ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
   </si>
   <si>
-    <t>{0: ['huge fan', 'food', 'teenage daughter'], 1: ['staff here', 'orders'], 2: ['McDs'], 3: ['quality service', 'quality people'], 4: ['evening crew'], 5: [], 6: ['girls', 'staff', 'order'], 7: ['Great people', 'service']}</t>
-  </si>
-  <si>
-    <t>{0: ['fan = huge', 'food = fast', 'daughter = teenage'], 1: ['staff = friendly'], 2: ['McDs = good'], 3: [], 4: [], 5: [], 6: ['girls = joke', 'staff = go'], 7: ['service = great', 'people = great', 'service = excellent']}</t>
+    <t>{0: ['food'], 1: ['staff here'], 2: ['mcds'], 3: ['quality service', 'quality people'], 4: [], 5: [], 6: ['staff', 'order'], 7: ['great people', 'service']}</t>
+  </si>
+  <si>
+    <t>{0: [('food', 'fast')], 1: [], 2: [('mcds', 'good')], 3: [('staff', 'enjoy'), ('staff', 'find')], 4: [], 5: [], 6: [('staff', 'go')], 7: [('people', 'great'), ('service', 'great'), ('service', 'excellent')]}</t>
   </si>
   <si>
     <t>Worst McDonaldÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿</t>
   </si>
   <si>
-    <t>{0: ['Worst McDonald']}</t>
-  </si>
-  <si>
-    <t>{0: ['McDonald = bad']}</t>
+    <t>{0: ['worst mcdonald']}</t>
+  </si>
+  <si>
+    <t>{0: [('mcdonald', 'bad')]}</t>
   </si>
   <si>
     <t>6 months ago</t>
@@ -170,28 +170,28 @@
 My husband went to get it, she finished her task then handed it to him without a word or smile or anything.</t>
   </si>
   <si>
-    <t>{0: ['quick breakfast'], 1: ['long drive thru'], 2: ['food items', 'drinks'], 3: ['food item'], 4: ['lady'], 5: ['husband', 'task', 'smile']}</t>
-  </si>
-  <si>
-    <t>{0: ['breakfast = quick'], 1: ['stopped = not crowded', 'drive = long'], 2: [], 3: [], 4: ['lady = ignore'], 5: ['husband = go']}</t>
+    <t>{0: [], 1: ['long drive thru'], 2: ['food items'], 3: ['food item'], 4: [], 5: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('drive', 'long')], 2: [], 3: [], 4: [], 5: []}</t>
   </si>
   <si>
     <t>The morning crew seems fast and efficient. Night crew is a whole different experience, lines down the street, hour long waits. If this was a one time occurrence it wouldn't be so bad but this is a nightly problem. Beyond this the staff is so highly rude you leave wanting to crash your car through the building. Don't forget they will mistake your order almost every single time as well and serve it to you cold.</t>
   </si>
   <si>
-    <t>{0: ['morning crew'], 1: ['Night crew', 'different experience', 'lines', 'long waits'], 2: ['time occurrence', 'nightly problem'], 3: ['staff', 'car'], 4: ['order', 'single time']}</t>
-  </si>
-  <si>
-    <t>{0: ['crew = seem'], 1: ['lines = whole', 'lines = different', 'experience = whole', 'experience = different', 'waits = long'], 2: ['problem = nightly'], 3: ['staff = rude'], 4: ['time = single']}</t>
+    <t>{0: ['morning crew'], 1: ['night crew', 'different experience', 'long waits'], 2: ['time occurrence'], 3: ['staff'], 4: ['order', 'single time']}</t>
+  </si>
+  <si>
+    <t>{0: [('crew', 'seem')], 1: [('experience', 'whole'), ('experience', 'different'), ('wait', 'long')], 2: [], 3: [('staff', 'leave')], 4: [('staff', 'mistake'), ('time', 'single')]}</t>
   </si>
   <si>
     <t>Today, i was disappointed in that restaurant #11853 did not get me my FULL order, meaning I did not receive my condiments for my big breakfast with hot cakes. No butter, no syrup, and no utensils. Luckily this was a hiccup and not a regular thing. Oh, and the egg was half the size of the sausage.</t>
   </si>
   <si>
-    <t>{0: ['FULL order', 'condiments', 'big breakfast', 'cakes'], 1: ['syrup', 'utensils'], 2: ['regular thing'], 3: ['egg']}</t>
-  </si>
-  <si>
-    <t>{0: ['11853 = get', 'order = full', 'breakfast = big', 'cakes = hot'], 1: [], 2: ['thing = regular'], 3: []}</t>
+    <t>{0: ['full order'], 1: [], 2: [], 3: []}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'full')], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
     <t>5 months ago</t>
@@ -200,37 +200,37 @@
     <t>Ordered food burger wrong and left out part of the order also. One of the drink cup lid not fattened. Poor service girl handing order at window on January 7, 2023 at 1pm.</t>
   </si>
   <si>
-    <t>{0: ['food burger', 'part'], 1: ['drink cup lid'], 2: ['Poor service girl', 'order']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['One = fatten'], 2: ['girl = poor', 'girl = hand']}</t>
+    <t>{0: ['food burger', 'part'], 1: ['drink cup lid'], 2: ['poor service girl', 'order']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('one', 'fatten')], 2: []}</t>
   </si>
   <si>
     <t>This was a dine in experience. The tables were all dirty &amp; we did not get our food after waiting 35 minutes. Chicken sandwich was burnt.</t>
   </si>
   <si>
-    <t>{0: [], 1: ['tables', 'food', 'minutes'], 2: []}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['tables = dirty'], 2: []}</t>
+    <t>{0: [], 1: ['food'], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('table', 'get')], 2: []}</t>
   </si>
   <si>
     <t>The line wS extremely big and was moving very slowly, plus they were out of apple pies and strawberry cream pies, but they gave me substitute cinnabun, the staff was very apologetic for being slow &amp; they were out of pies, but it was middle of the night and they were extremely under-staffed.</t>
   </si>
   <si>
-    <t>{0: ['line', 'apple pies', 'strawberry cream pies', 'substitute cinnabun', 'staff']}</t>
-  </si>
-  <si>
-    <t>{0: ['line = move', 'staff = apologetic']}</t>
+    <t>{0: ['line', 'staff']}</t>
+  </si>
+  <si>
+    <t>{0: [('line', 'move'), ('line', 'give')]}</t>
   </si>
   <si>
     <t>The boy who attended me made me wait and when he saw that the drink was wrong he threw the bag of food at me with a grimace. So disappointed!</t>
   </si>
   <si>
-    <t>{0: ['boy', 'drink', 'bag'], 1: []}</t>
-  </si>
-  <si>
-    <t>{0: ['boy = make', 'drink = wrong', 'boy = throw'], 1: []}</t>
+    <t>{0: ['boy', 'drink'], 1: []}</t>
+  </si>
+  <si>
+    <t>{0: [('boy', 'attend'), ('boy', 'make'), ('boy', 'wait'), ('boy', 'see'), ('boy', 'throw')], 1: []}</t>
   </si>
   <si>
     <t>7 months ago</t>
@@ -239,19 +239,19 @@
     <t>I am not happy at all today I went and bought 4 Strawberry Banana smoothies and and 2 hash browns and my smoothies tasted like straight ice and water smh. And I am very disappointed in there service my smoothie should never taste like that never especially the fact I bought it for not only me but my kids. I need someone to contact me from corporate or something. I am not happy at all waste of moneyÃÂ¯ÃÂ¿ÃÂ½</t>
   </si>
   <si>
-    <t>{0: ['smoothies', 'hash browns', 'smoothies', 'straight ice'], 1: ['smoothie'], 2: ['fact especially'], 3: [], 4: []}</t>
-  </si>
-  <si>
-    <t>{0: ['smh = straight', 'ice = straight'], 1: ['smoothie = taste'], 2: [], 3: [], 4: []}</t>
+    <t>{0: [], 1: ['smoothie'], 2: [], 3: [], 4: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('smoothie', 'taste')], 2: [('smoothie', 'buy')], 3: [('smoothie', 'need')], 4: []}</t>
   </si>
   <si>
     <t>The staff seems to always be different which makes ordering sometimes a little difficult because they are in a state of perpetual learning which can also lead to waiting a bit longer but the lobby is always clean as well as the bathrooms</t>
   </si>
   <si>
-    <t>{0: ['staff', 'perpetual learning', 'lobby']}</t>
-  </si>
-  <si>
-    <t>{0: ['staff = seem', 'learning = perpetual', 'lobby = clean']}</t>
+    <t>{0: ['staff', 'perpetual learning']}</t>
+  </si>
+  <si>
+    <t>{0: [('staff', 'seem'), ('staff', 'make'), ('learning', 'perpetual'), ('staff', 'lead')]}</t>
   </si>
   <si>
     <t>10 months ago</t>
@@ -263,10 +263,10 @@
 I didn't want to complain but this was intolerable.</t>
   </si>
   <si>
-    <t>{0: ['experience', 'order taker'], 1: ['drive thru', 'employee'], 2: ['order', 'other cars', 'order'], 3: ['more item'], 4: [], 5: [], 6: ['other car', 'order', 'time either'], 7: [], 8: [], 9: [], 10: ['name', 'review'], 11: ['credit card'], 12: ['card'], 13: [], 14: ['order'], 15: [], 16: ['hand several times'], 17: ['window', 'receipt', 'next window'], 18: [], 19: ['next window', 'food', 'name'], 20: ['receipt'], 21: []}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['employee = ask'], 2: ['cars = other', 'cars = place'], 3: ['item = more'], 4: [], 5: [], 6: ['car = other'], 7: [], 8: [], 9: [], 10: ['name = put'], 11: [], 12: [], 13: [], 14: [], 15: [], 16: ['times = several'], 17: ['window = next'], 18: [], 19: [], 20: ['receipt = state'], 21: []}</t>
+    <t>{0: ['experience', 'order taker'], 1: ['drive thru', 'employee'], 2: ['order', 'order'], 3: [], 4: [], 5: [], 6: ['order', 'time either'], 7: [], 8: [], 9: [], 10: [], 11: [], 12: [], 13: [], 14: ['order'], 15: [], 16: [], 17: ['window', 'next window'], 18: [], 19: ['next window', 'food'], 20: [], 21: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('employee', 'ask'), ('employee', 'want')], 2: [('employee', 'keep')], 3: [], 4: [], 5: [], 6: [], 7: [], 8: [], 9: [], 10: [], 11: [], 12: [], 13: [], 14: [], 15: [], 16: [('time', 'several')], 17: [('window', 'next')], 18: [], 19: [], 20: [], 21: []}</t>
   </si>
   <si>
     <t>4 years ago</t>
@@ -275,10 +275,10 @@
     <t>Meh.. just meh. When I finally get the correct order, it is generally tasty. I'm a picky eater, and have found ways to navigate the menu to get items I like. Worked in the service industry for years as a server, bartender, and trainer. Taking and fulfilling orders is NOT hard, tedious at times though. I only go here when I see they are not busy, in hope that my order is correct when I go to leave. In the 10 times that I have been here in the past past year, I have only had 1 order that was perfectly correct. Just ONE, not an exaggeration. That one order was just 2 large fries and nothing else. Though I will mention that when I got home and pulled them out of the bag, they were hardly what you'd call filled, (nor did I enjoy any on the 3 minute drive home) so little so that I even sent a picture and post to McDonald's on Facebook, at least the few were hot. The evening staff is very pleasant, but the morning staff leaves a lot to be desired, as well as thinking that they can talk negatively about people in Spanish out in the open which, being a light skinned Puerto Rican, I understand perfectly. I have submitted several complaints and NEVER received a call or email back. I just don't go here anymore to avoid the stress of paying money for something that is most likely wrong.</t>
   </si>
   <si>
-    <t>{0: ['meh just'], 1: ['order'], 2: ['eater', 'ways', 'menu', 'items'], 3: ['service industry', 'bartender', 'trainer'], 4: ['orders'], 5: ['order'], 6: ['past year', 'order'], 7: [], 8: ['order', 'large fries'], 9: ['minute drive home'], 10: ['picture', 'post'], 11: ['evening staff', 'morning staff', 'lot'], 12: ['several complaints', 'call', 'email'], 13: ['stress', 'money']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['order = correct'], 2: ['eater = picky'], 3: [], 4: [], 5: ['order = correct'], 6: ['year = past', 'year = past'], 7: [], 8: ['fries = large', 'nothing = large'], 9: [], 10: ['few = hot'], 11: ['staff = pleasant', 'staff = leave'], 12: ['complaints = several'], 13: []}</t>
+    <t>{0: ['meh just'], 1: ['order'], 2: [], 3: ['service industry'], 4: [], 5: ['order'], 6: ['order'], 7: [], 8: ['order'], 9: ['minute drive home'], 10: [], 11: ['evening staff', 'morning staff'], 12: [], 13: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('order', 'correct')], 2: [], 3: [], 4: [], 5: [('order', 'go')], 6: [('order', 'have')], 7: [], 8: [('fry', 'large')], 9: [('order', 'mention'), ('order', 'get'), ('order', 'call'), ('order', 'enjoy')], 10: [('order', 'send')], 11: [('staff', 'leave'), ('staff', 'talk'), ('staff', 'understand')], 12: [('staff', 'submit')], 13: [('staff', 'go')]}</t>
   </si>
   <si>
     <t>Just needed caffeine. The staff at the drive thru just shoved the drink in my hands. Not very professional.</t>
@@ -287,7 +287,7 @@
     <t>{0: ['caffeine'], 1: ['staff thru', 'drink'], 2: []}</t>
   </si>
   <si>
-    <t>{0: [], 1: ['staff = shove'], 2: []}</t>
+    <t>{0: [], 1: [('staff', 'shove')], 2: []}</t>
   </si>
   <si>
     <t>8 months ago</t>
@@ -296,10 +296,10 @@
     <t>This is consistently the worst meal you will pay for. Microwaved nuggets, cold fries and a 30 minute wait. What more can you ask for? Dont go here ever! Your better off going hungry or giving the meal you payed for to the homeless by the donation box behind the drive thru.</t>
   </si>
   <si>
-    <t>{0: ['meal'], 1: ['fries', 'minute wait'], 2: [], 3: [], 4: ['meal', 'donation box']}</t>
-  </si>
-  <si>
-    <t>{0: ['meal = bad'], 1: ['fries = cold', 'wait = cold'], 2: [], 3: [], 4: []}</t>
+    <t>{0: ['meal'], 1: ['minute wait'], 2: [], 3: [], 4: ['meal', 'donation box']}</t>
+  </si>
+  <si>
+    <t>{0: [('meal', 'bad')], 1: [('fry', 'cold'), ('wait', 'cold')], 2: [], 3: [], 4: []}</t>
   </si>
   <si>
     <t>4 months ago</t>
@@ -317,10 +317,10 @@
     <t>McDonaldÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s is proud to own the most broken ice cream machines on the planet. When I asked at the drive through if they had ice cream the lady replied ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½naÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
   </si>
   <si>
-    <t>{0: ['ice cream machines'], 1: ['ice cream', 'lady']}</t>
-  </si>
-  <si>
-    <t>{0: ['McDonalds = proud', 'machines = broken'], 1: ['lady = reply']}</t>
+    <t>{0: ['ice cream machines'], 1: ['ice cream']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('mcdonalds', 'ask'), ('mcdonalds', 'have')]}</t>
   </si>
   <si>
     <t>With all the new upgrades everything looks great and clean great staff</t>
@@ -329,10 +329,10 @@
     <t>{0: ['new upgrades', 'staff']}</t>
   </si>
   <si>
-    <t>{0: ['upgrades = new', 'staff = great', 'staff = great']}</t>
-  </si>
-  <si>
-    <t>DoesnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿</t>
+    <t>{0: [('upgrade', 'new'), ('staff', 'great'), ('staff', 'great')]}</t>
+  </si>
+  <si>
+    <t>DoesnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½Ã</t>
   </si>
   <si>
     <t>{0: []}</t>
@@ -341,10 +341,10 @@
     <t>Yet another McDonald's with horrible service and lazy employees. I mean c'mon do they intentionally hire unqualified people???</t>
   </si>
   <si>
-    <t>{0: ['McDonald Yet', 'service', 'employees'], 1: ['people']}</t>
-  </si>
-  <si>
-    <t>{0: ['service = horrible', 'employees = horrible', 'employees = lazy'], 1: ['people = unqualified']}</t>
+    <t>{0: ['mcdonald yet', 'service'], 1: ['people']}</t>
+  </si>
+  <si>
+    <t>{0: [('service', 'horrible'), ('employee', 'lazy')], 1: [('people', 'unqualified')]}</t>
   </si>
   <si>
     <t>3 years ago</t>
@@ -356,7 +356,7 @@
     <t>{0: ['last time'], 1: [], 2: ['plain sausage biscuit', 'double quarter pounder'], 3: []}</t>
   </si>
   <si>
-    <t>{0: ['time = last'], 1: [], 2: ['sausage = plain', 'quarter = double'], 3: []}</t>
+    <t>{0: [('time', 'last')], 1: [], 2: [('sausage', 'plain'), ('quarter', 'double')], 3: []}</t>
   </si>
   <si>
     <t>2 years ago</t>
@@ -377,10 +377,10 @@
 Look McDonald's if I wanted a breakfast deluxe I wouldn't have shown up at 2:30 in the morning thank you.</t>
   </si>
   <si>
-    <t>{0: ['location'], 1: ['orders', 'people', 'parking lot', 'dinner food'], 2: ['multiple times', 'parking lot', 'order menu'], 3: ['breakfast deluxe']}</t>
-  </si>
-  <si>
-    <t>{0: ['location = wack'], 1: ['people = sit', 'parking = get'], 2: ['times = multiple', 'menu = change'], 3: ['McDonald = show']}</t>
+    <t>{0: ['location'], 1: ['people', 'parking lot', 'dinner food'], 2: ['parking lot', 'order menu'], 3: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('location', 'stop'), ('people', 'sit'), ('people', 'get')], 2: [('people', 'go'), ('time', 'multiple'), ('people', 'do')], 3: [('mcdonald', 'want'), ('mcdonald', 'show')]}</t>
   </si>
   <si>
     <t>They did not honor there advertised price. This is extra pickles.</t>
@@ -389,16 +389,16 @@
     <t>{0: ['price'], 1: ['extra pickles']}</t>
   </si>
   <si>
-    <t>{0: [], 1: ['pickles = extra']}</t>
+    <t>{0: [], 1: [('pickle', 'extra')]}</t>
   </si>
   <si>
     <t>Just spent 10 minutes waiting at this McDonald's . According to Google they're open 24/7. Finally we pull up to the window to see if anyone was there, sure enough one employee seated in the lobby and another at the window. She told me they were closed. Whoever these two are they need to be replaced. Get it together McDonald's. You're a corporate power house and you have a reputation to keep. One of the most unprofessional experiences I've ever had with fast food. 0/10 would not recomend this location.</t>
   </si>
   <si>
-    <t>{0: ['minutes'], 1: ['open 24/7'], 2: [], 3: [], 4: [], 5: ['McDonald'], 6: ['corporate power house', 'reputation'], 7: ['unprofessional experiences', 'food'], 8: ['location']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['24/7 = open'], 2: [], 3: [], 4: [], 5: [], 6: ['house = corporate'], 7: ['experiences = unprofessional', 'food = fast'], 8: ['0/10 = recomend']}</t>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: ['mcdonald'], 6: [], 7: ['food'], 8: ['location']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [], 6: [], 7: [('experience', 'unprofessional'), ('food', 'fast')], 8: []}</t>
   </si>
   <si>
     <t>We hit it off pretty good in the beginning everything was great but that didnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t last long. I mean the service is fast but with attitude an</t>
@@ -407,16 +407,13 @@
     <t>{0: [], 1: ['service']}</t>
   </si>
   <si>
-    <t>{0: ['last = great', 'hit = great', 'was = great'], 1: ['service = fast', 'service = with']}</t>
-  </si>
-  <si>
     <t xml:space="preserve">This location is a horrible store to work for. The General Manger Omar Delgado  doesnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t know how to run a store efficiently. The Supervisor, Eduardo doesnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t care how itÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s ran either.  As someone who used to work here at the Manger </t>
   </si>
   <si>
     <t>{0: ['location', 'store'], 1: ['store'], 2: [], 3: []}</t>
   </si>
   <si>
-    <t>{0: ['store = horrible'], 1: ['Delgado = know'], 2: ['Supervisor = care', 'Eduardo = care'], 3: []}</t>
+    <t>{0: [('store', 'horrible')], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
     <t>This is 3rd time I got this ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
@@ -425,7 +422,7 @@
     <t>{0: ['3rd time']}</t>
   </si>
   <si>
-    <t>{0: ['time = 3rd']}</t>
+    <t>{0: [('time', '3rd')]}</t>
   </si>
   <si>
     <t>The staff are very friendly and they do their job perfectly</t>
@@ -434,16 +431,16 @@
     <t>{0: ['staff', 'job']}</t>
   </si>
   <si>
-    <t>{0: ['staff = friendly']}</t>
+    <t>{0: [('staff', 'do')]}</t>
   </si>
   <si>
     <t>Awesome service! Food hot!  Best ever</t>
   </si>
   <si>
-    <t>{0: ['Awesome service'], 1: [], 2: []}</t>
-  </si>
-  <si>
-    <t>{0: ['service = awesome'], 1: [], 2: []}</t>
+    <t>{0: ['awesome service'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('service', 'awesome')], 1: [], 2: []}</t>
   </si>
   <si>
     <t>Went through the drive through ordered a large fry and two chicken deluxe sandwiches
@@ -452,40 +449,40 @@
 They said they would fix it after having to pay a second time for the lettuce and tomatoÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ then when I got the order it was still a spicey chicken sandwich INSIDE a deluxe crispy chicken b</t>
   </si>
   <si>
-    <t>{0: ['large fry', 'deluxe sandwiches', 'pay window', 'read back', 'spicey chicken sandwiches', 'deluxe crispy chicken sandwich'], 1: ['second time', 'tomato', 'order', 'spicey chicken sandwich', 'deluxe crispy chicken']}</t>
-  </si>
-  <si>
-    <t>{0: ['fry = large', 'sandwiches = large', 'sandwiches = deluxe', 'sandwiches = spicey'], 1: ['time = second', 'crispy = deluxe']}</t>
+    <t>{0: ['large fry', 'deluxe sandwiches', 'pay window', 'read back', 'spicey chicken sandwiches', 'deluxe crispy chicken sandwich'], 1: ['second time', 'order', 'spicey chicken sandwich', 'deluxe crispy chicken']}</t>
+  </si>
+  <si>
+    <t>{0: [('fry', 'large'), ('sandwich', 'deluxe'), ('sandwich', 'spicey')], 1: [('deluxe', 'say'), ('deluxe', 'fix'), ('time', 'second'), ('deluxe', 'get')]}</t>
   </si>
   <si>
     <t>11 months ago</t>
   </si>
   <si>
-    <t>If you didnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
-  </si>
-  <si>
-    <t>{0: ['minutes', 'few orders', 'normal menu']}</t>
-  </si>
-  <si>
-    <t>{0: ['orders = few', 'I = able', 'd = able', 'menu = normal', 'br = disgusting']}</t>
+    <t>If you didnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t take 15 minutes to take a few orders IÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½d be able to order off your normal menu instead of the disgusting br</t>
+  </si>
+  <si>
+    <t>{0: ['few orders', 'normal menu']}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'few'), ('menu', 'normal')]}</t>
   </si>
   <si>
     <t>This is the WORST McDonald's EVER, I don't come here often because when I do my order is wrong EVERY TIME.  Today 2/25/22 1130am 1 the drive thru person could barely hear me and I was almost yelling 2 I get to the next window after paying and I'm asked what did you order?? I tell them at the end of me repeating my order I now have your entire staff looking CONFUSED AS HELL like I just dropped outta the sky now I'm being asked did I pay? Are you sure you ordered at the speaker? Now all of ya'll wear head sets except for the cooks the worst leadership I've ever seen</t>
   </si>
   <si>
-    <t>{0: ['WORST McDonald', 'order'], 1: ['drive thru person', 'next window'], 2: [], 3: ['order', 'entire staff'], 4: ['sky'], 5: [], 6: ['head sets', 'leadership']}</t>
-  </si>
-  <si>
-    <t>{0: ['McDonald = bad'], 1: ['1130am = hear', 'window = next'], 2: [], 3: ['staff = entire', 'staff = look'], 4: [], 5: [], 6: ['leadership = bad']}</t>
+    <t>{0: ['worst mcdonald', 'order'], 1: ['drive thru person', 'next window'], 2: [], 3: ['order', 'entire staff'], 4: [], 5: [], 6: []}</t>
+  </si>
+  <si>
+    <t>{0: [('mcdonald', 'bad')], 1: [('window', 'next')], 2: [], 3: [('staff', 'entire'), ('staff', 'look')], 4: [('staff', 'drop'), ('staff', 'pay')], 5: [('staff', 'order')], 6: [('staff', 'wear'), ('staff', 'see')]}</t>
   </si>
   <si>
     <t>Me and my girlfriend came tonight to pick up our food after 11pm for a mobile order, they need a better system if you are walking on foot. The food tasted great, loved the McDonald's deal ordering from the app.</t>
   </si>
   <si>
-    <t>{0: ['food', 'mobile order', 'system'], 1: ['food', 'deal']}</t>
-  </si>
-  <si>
-    <t>{0: ['order = mobile', 'system = well'], 1: ['food = taste']}</t>
+    <t>{0: ['food', 'mobile order'], 1: ['food', 'deal']}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'mobile')], 1: [('food', 'taste')]}</t>
   </si>
   <si>
     <t>Been frequenting this location for a few years.Morning,mid-day and night,the food is always hot,fresh and served with a smile.</t>
@@ -494,25 +491,22 @@
     <t>{0: ['location', 'few years'], 1: ['- day', 'night', 'food']}</t>
   </si>
   <si>
-    <t>{0: ['years = few'], 1: ['food = hot', 'food = fresh']}</t>
+    <t>{0: [('year', 'few')], 1: []}</t>
   </si>
   <si>
     <t>The drinks were watered down and the employee was downright rude when asked to replace the drinks.!!</t>
   </si>
   <si>
-    <t>{0: ['employee', 'drinks']}</t>
-  </si>
-  <si>
-    <t>{0: ['employee = rude']}</t>
+    <t>{0: ['employee']}</t>
   </si>
   <si>
     <t>I ordered a Large fry buy after arriving to my destination I saw they did not fill the carton up.  They gave me a small portion for what I paid for.  This is not right and management needs to correct this.  Stealing from customers is plain wrong.  When ordering a large, they expect to get what should come in a large.  I noticed after my bad experience that your reviews are low.  In order order to create a good business, giving people an exceptional experience should be your goal not the opposite.</t>
   </si>
   <si>
-    <t>{0: ['Large fry buy', 'carton'], 1: ['small portion'], 2: ['management'], 3: [], 4: [], 5: ['experience', 'reviews'], 6: ['order order', 'business', 'experience']}</t>
-  </si>
-  <si>
-    <t>{0: ['buy = large'], 1: ['portion = small'], 2: ['management = need'], 3: [], 4: [], 5: ['experience = bad', 'reviews = low'], 6: ['business = good', 'experience = exceptional']}</t>
+    <t>{0: ['large fry buy'], 1: [], 2: [], 3: [], 4: [], 5: ['experience'], 6: ['order order', 'experience']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [('experience', 'bad')], 6: [('experience', 'exceptional')]}</t>
   </si>
   <si>
     <t>Will not answer my call. Messed up my order 4times in and hour!</t>
@@ -524,55 +518,55 @@
     <t>Slow always have wait for my food and have to go back in to get it fixed.  No one ever iles or has a none fake smile. No welcome to McDonald's or have a great day especially in drive through . And if you do say something's wrong you get a major attitude especially from the shift manager guy tall black guy .  ( Sorry don't know his name )</t>
   </si>
   <si>
-    <t>{0: [], 1: ['one', 'iles ever', 'smile'], 2: ['day'], 3: ['major attitude', 'shift manager guy', 'black guy'], 4: ['name']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['smile = fake'], 2: ['day = great'], 3: ['attitude = major', 'guy = tall', 'guy = black'], 4: []}</t>
+    <t>{0: [], 1: ['one', 'iles ever'], 2: ['day'], 3: ['shift manager guy', 'black guy'], 4: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [('day', 'great')], 3: [('one', 'say'), ('one', 'get'), ('guy', 'tall'), ('guy', 'black')], 4: []}</t>
   </si>
   <si>
     <t>Horrible service worker with a stank attitude for no reason working at the window mute with an attitude mad because she is miserable at work . They mess up the order and then donÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t answer the phone itÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s ridiculous. Found a long hair in my daughters happy meal fries and then the extra fry was missing from her meal and t</t>
   </si>
   <si>
-    <t>{0: ['Horrible service worker', 'stank attitude', 'window mute'], 1: ['order', 'phone'], 2: ['long hair', 'meal fries', 'extra fry']}</t>
-  </si>
-  <si>
-    <t>{0: ['worker = horrible', 'attitude = stank'], 1: [], 2: ['hair = long', 'meal = happy', 'fry = extra']}</t>
+    <t>{0: ['horrible service worker', 'stank attitude', 'window mute'], 1: ['order'], 2: ['long hair', 'meal fries', 'extra fry']}</t>
+  </si>
+  <si>
+    <t>{0: [('attitude', 'stank')], 1: [], 2: [('meal', 'happy'), ('fry', 'extra')]}</t>
   </si>
   <si>
     <t>Normally this location does pretty good, but last night was absolutely ridiculous. I sat in the drive thru for almost an hour waiting to get my order taken, the line was wrapped almost TWICE around the building, and finally I gave up and tried driving up to the window to give them my order since i was next in line. When i got to the window, they told me they couldn't take it and I'd have to go back around. I told them I'd like to put in my order here since I've been waiting all this time, and they proceeded to still refuse and that it's my fault for waiting in the second lane that they claimed was closed and had a sign out. The second lane was open, and the "sign" they were talking about was a wet floor sign they had placed right next to the drive-thru menu. I told them the lane looked open from our side and they still proceeded to argue with me, and then slammed the drive thru window shut. I've never received such deplorable customer service in my life, and if any managers are reading this, I highly suggest firing the two workers from last night.</t>
   </si>
   <si>
-    <t>{0: ['location', 'last night'], 1: ['order', 'order'], 2: [], 3: [], 4: ['order', 'second lane', 'sign'], 5: ['second lane', 'sign', 'wet floor sign', 'thru menu'], 6: ['lane', 'window shut'], 7: ['customer service', 'managers', 'workers', 'last night']}</t>
-  </si>
-  <si>
-    <t>{0: ['night = last', 'night = ridiculous'], 1: ['order = take'], 2: [], 3: [], 4: ['lane = second'], 5: ['lane = second', 'lane = open', 'floor = wet'], 6: ['lane = look'], 7: ['service = such', 'service = deplorable', 'managers = read', 'night = last']}</t>
+    <t>{0: ['location', 'last night'], 1: ['order', 'order'], 2: [], 3: [], 4: ['order', 'second lane', 'sign'], 5: ['second lane', 'sign', 'wet floor sign', 'thru menu'], 6: ['lane', 'window shut'], 7: ['customer service', 'last night']}</t>
+  </si>
+  <si>
+    <t>{0: [('night', 'last')], 1: [('location', 'sit'), ('order', 'take'), ('order', 'give')], 2: [('order', 'get'), ('order', 'tell'), ('order', 'take')], 3: [('order', 'have')], 4: [('order', 'tell'), ('order', 'like'), ('order', 'wait'), ('order', 'proceed'), ('lane', 'second'), ('order', 'claim'), ('order', 'close')], 5: [('lane', 'second'), ('lane', 'talk'), ('lane', 'place')], 6: [('lane', 'tell'), ('lane', 'look'), ('lane', 'proceed')], 7: [('lane', 'receive'), ('service', 'such'), ('service', 'deplorable'), ('manager', 'read'), ('manager', 'suggest'), ('night', 'last')]}</t>
   </si>
   <si>
     <t>I went to this location tonight to see if they could give me the Oreo Mcflurry that a different McDonaldÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s had forgotten earlier they completely refused. Unbelievable.. ItÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s ice creamÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
   </si>
   <si>
-    <t>{0: ['location tonight'], 1: [], 2: ['ice cream']}</t>
-  </si>
-  <si>
-    <t>{0: ['went = give', 'McDonalds = forget'], 1: [], 2: []}</t>
+    <t>{0: ['location tonight'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('mcdonalds', 'forget'), ('mcdonalds', 'refuse')], 1: [], 2: []}</t>
   </si>
   <si>
     <t>Rude customer service, unprofessional attitude, overcooked food, no complimentary items for screwing up our orders. I don't understand how you can keep your job when there is so many negative reviews. I vow to never eat here again. I would rather eat a cold can of baked beans...</t>
   </si>
   <si>
-    <t>{0: ['Rude customer service', 'unprofessional attitude', 'overcooked food', 'items', 'orders'], 1: ['job', 'reviews'], 2: [], 3: ['can', 'baked beans']}</t>
-  </si>
-  <si>
-    <t>{0: ['attitude = rude', 'service = rude', 'food = rude', 'attitude = unprofessional', 'food = unprofessional', 'food = overcooked', 'items = complimentary'], 1: ['reviews = many', 'reviews = negative'], 2: [], 3: ['can = cold', 'beans = baked']}</t>
+    <t>{0: ['rude customer service', 'overcooked food'], 1: [], 2: [], 3: ['can']}</t>
+  </si>
+  <si>
+    <t>{0: [('food', 'rude'), ('service', 'rude'), ('food', 'unprofessional'), ('food', 'overcooked')], 1: [], 2: [], 3: [('can', 'cold')]}</t>
   </si>
   <si>
     <t>Representative was very rude and disrespectful,  refused fulfilling my order and simply hung up on me on the drive through window... never was I so disappointed at that location before. Manager pretended like nothing even happened.</t>
   </si>
   <si>
-    <t>{0: ['order'], 1: [], 2: ['Manager']}</t>
-  </si>
-  <si>
-    <t>{0: ['Representative = rude', 'Representative = disrespectful'], 1: [], 2: ['Manager = pretend']}</t>
+    <t>{0: ['order'], 1: [], 2: ['manager']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [('manager', 'pretend')]}</t>
   </si>
   <si>
     <t>They got our order correct and didn't cut me off before I had finished ordering our food at the speaker. I could actually understand our order taker. I don't know if it really gets any better than that at a fast food place anymore.</t>
@@ -581,7 +575,7 @@
     <t>{0: ['order', 'food'], 1: ['order taker'], 2: ['food place']}</t>
   </si>
   <si>
-    <t>{0: [], 1: [], 2: ['place = fast']}</t>
+    <t>{0: [('order', 'finish')], 1: [('order', 'understand')], 2: [('order', 'know'), ('order', 'get'), ('place', 'fast')]}</t>
   </si>
   <si>
     <t>Good quick drive through service.  Was a long line but went very quickly.</t>
@@ -590,7 +584,7 @@
     <t>{0: ['quick drive'], 1: ['long line']}</t>
   </si>
   <si>
-    <t>{0: ['drive = good', 'drive = quick'], 1: ['line = long']}</t>
+    <t>{0: [('drive', 'good'), ('drive', 'quick')], 1: [('line', 'long')]}</t>
   </si>
   <si>
     <t>Yup. ItÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s McDona</t>
@@ -599,28 +593,28 @@
     <t>I go here all the time. Great staff.. NVR get my food wrong it's just always a line wrapped around lol that's why they ain't 5 stars. Most def customer service is better then the food but hey I just go for my kids because they love it so why not! Good customer service guys! Makes all the difference</t>
   </si>
   <si>
-    <t>{0: [], 1: ['Great staff'], 2: ['food'], 3: [], 4: ['def customer service'], 5: [], 6: ['Good customer service guys'], 7: ['difference']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['staff = great'], 2: ['NVR = get'], 3: [], 4: ['service = Most', 'service = def', 'service = better'], 5: [], 6: ['guys = good'], 7: []}</t>
+    <t>{0: [], 1: ['great staff'], 2: ['food'], 3: [], 4: ['def customer service'], 5: [], 6: ['good customer service guys'], 7: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('staff', 'great')], 2: [], 3: [], 4: [('service', 'most'), ('service', 'def')], 5: [('service', 'go'), ('service', 'love')], 6: [], 7: []}</t>
   </si>
   <si>
     <t>I went to pick up food from the restaurant at late night through drive through. I was told to wait near the door and I will be getting the order but even after waiting 15 minutes no one came with the food. Orders are already assigned and even after coming through drive through it takes more than half an hour to get it which is not good. Lots of people behind me got the food but no one cared about the driver who is already waiting from long time. Thank you</t>
   </si>
   <si>
-    <t>{0: ['food', 'late night', 'drive through'], 1: ['order', 'minutes', 'one'], 2: ['hour'], 3: ['Lots', 'food', 'one', 'long time'], 4: []}</t>
-  </si>
-  <si>
-    <t>{0: ['night = late'], 1: ['one = come'], 2: [], 3: ['Lots = get', 'one = care', 'time = long'], 4: []}</t>
+    <t>{0: ['food', 'late night', 'drive through'], 1: ['order', 'one'], 2: ['hour'], 3: ['food', 'one', 'long time'], 4: []}</t>
+  </si>
+  <si>
+    <t>{0: [('night', 'late')], 1: [('one', 'come')], 2: [('one', 'take')], 3: [('one', 'care'), ('time', 'long')], 4: []}</t>
   </si>
   <si>
     <t>OPEN 24HRS all the darn time!!  If there are 24 hours in every day and then 7 days in a week then that means this place is open eleventeen million hours a year.  I dont even know how they find people to work here I mean how do they shower or brush their teeth or change clothes if they are always there.... I think I may have an idea: they are robots.  Or clones, like this example that's Dolly the sheep she's pretty hot NGL.</t>
   </si>
   <si>
-    <t>{0: ['darn time'], 1: ['place'], 2: ['people'], 3: ['teeth', 'clothes'], 4: ['idea'], 5: ['clones']}</t>
-  </si>
-  <si>
-    <t>{0: ['time = darn'], 1: ['place = open'], 2: ['people = work'], 3: [], 4: [], 5: []}</t>
+    <t>{0: ['darn time'], 1: ['place'], 2: ['people'], 3: [], 4: [], 5: []}</t>
+  </si>
+  <si>
+    <t>{0: [('time', 'darn')], 1: [], 2: [('place', 'know'), ('place', 'find'), ('people', 'work')], 3: [('people', 'mean'), ('people', 'shower')], 4: [('people', 'think'), ('people', 'have')], 5: []}</t>
   </si>
   <si>
     <t>It was late, order was wrong, person taking order needs to slow down,</t>
@@ -629,126 +623,117 @@
     <t>{0: ['order', 'person', 'order']}</t>
   </si>
   <si>
-    <t>{0: ['order = wrong', 'person = need']}</t>
+    <t>{0: [('person', 'need')]}</t>
   </si>
   <si>
     <t>The manager IS RUDE at 13749 183 research Blvd.in north Austin TX. HAD TO GO BACK INTO THE  DINER  3 TIMES AND THE 3RD TIME THE MANAGER DIDNT EVEN ACKOWLEDGE WE WERE EVEN THERE.. DISCRIPTION OF SAID MANAGER SPANISH ABOUT 5 FT TALL AND HAD LONG BLONDOISH HAIR PULLED BACK INTO A PONY TAIL. READ PREVIOUS REVIEWS AND THRY WERE NOT GOOD
 NEED TO CHECK OUT WHAT IS GOING ON .</t>
   </si>
   <si>
-    <t>{0: ['manager'], 1: ['MANAGER DIDNT'], 2: ['TALL'], 3: ['PREVIOUS REVIEWS']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: [], 2: ['DISCRIPTION = SPANISH'], 3: ['REVIEWS = previous', 'NEED = good']}</t>
+    <t>{0: ['manager'], 1: ['manager didnt'], 2: [], 3: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: [('need', 'good')]}</t>
   </si>
   <si>
     <t>Never would come back here again my mother was asking for a coke and the lady became rude and said to her coworker in Spanish omg this fat women it hurt me that she said that and we know what she said so teach your employees how to speck properly in front of people</t>
   </si>
   <si>
-    <t>{0: ['mother', 'lady', 'women', 'employees']}</t>
-  </si>
-  <si>
-    <t>{0: ['mother = ask', 'lady = become', 'women = fat', 'and = hurt']}</t>
-  </si>
-  <si>
     <t>I placed an order... the young lady at the drive thru kept having issues getting the order correctly... I paid for my order... went to the second window.. was given a huge bag that almost broke through with stuff... I pulled up just a little bit to check my order:  noticed I was missing an item, fries, so I pulled around to let the lady at the first window know IÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½m missing something... she just dismissed me to the 2nd window... and the 2 ladies at the second window werenÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t the best either.  When I stated I drove back around because I was missing my fries.. I didnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t realize my receipt was in the bag to confirm my order.. found it and gave it to one of the ladies... the second lady, IÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½m guessing to be heard due to my inconvenience of my order not being correct, for her to take ownership for what possibly could of went wrong and show some compassion instead of being kind of prude ... after I received the fries the manager dismissed me with a condescending ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½</t>
   </si>
   <si>
-    <t>{0: ['order'], 1: ['young lady thru', 'issues', 'order'], 2: ['second window', 'huge bag'], 3: ['little bit just', 'order', 'item', 'lady', 'first window'], 4: [], 5: ['2nd window', 'ladies', 'second window'], 6: ['fries'], 7: ['receipt', 'order'], 8: ['second lady', 'ownership', 'compassion', 'fries', 'manager']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['lady = young', 'lady = keep'], 2: ['window = second', 'bag = huge'], 3: ['bit = little', 'window = first'], 4: [], 5: ['window = 2nd', 'window = second'], 6: [], 7: [], 8: ['lady = second', 'manager = dismiss']}</t>
+    <t>{0: ['order'], 1: ['young lady thru', 'order'], 2: ['second window'], 3: ['little bit just', 'order', 'lady', 'first window'], 4: [], 5: ['2nd window', 'second window'], 6: [], 7: ['order'], 8: ['second lady', 'manager']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('lady', 'young'), ('lady', 'keep')], 2: [('lady', 'pay'), ('window', 'second'), ('lady', 'break')], 3: [('lady', 'pull'), ('lady', 'miss'), ('lady', 'pull'), ('window', 'first')], 4: [('lady', 'miss')], 5: [('lady', 'dismiss'), ('window', '2nd'), ('window', 'second')], 6: [('lady', 'state'), ('lady', 'drive'), ('lady', 'miss')], 7: [('lady', 'realize')], 8: [('lady', 'second'), ('manager', 'dismiss')]}</t>
   </si>
   <si>
     <t>Never gotten my order wrong, employees seem to change a lot but they're consistently quick and nice. Also the prices here are lower than other locations, I don't know why but its a total welcome change haha.</t>
   </si>
   <si>
-    <t>{0: ['order', 'employees', 'lot'], 1: ['prices here', 'other locations', 'total welcome change']}</t>
-  </si>
-  <si>
-    <t>{0: ['employees = seem'], 1: ['prices = lower', 'locations = other', 'change = total']}</t>
+    <t>{0: ['order'], 1: ['prices here', 'total welcome change']}</t>
+  </si>
+  <si>
+    <t>{0: [('employee', 'seem')], 1: [('location', 'other'), ('change', 'total')]}</t>
   </si>
   <si>
     <t>They run out of fry containers and constantly forget sauces. The dining room is still closed for some reason so have fun getting back in line for a sauce. Sometimes the fries aren't great which is a huge part of McDonald's. Come on guys...</t>
   </si>
   <si>
-    <t>{0: ['fry containers', 'sauces'], 1: ['dining room', 'fun'], 2: ['fries', 'huge part'], 3: []}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['fun = get'], 2: ['fries = not great', 'part = huge'], 3: []}</t>
+    <t>{0: ['fry containers'], 1: [], 2: [], 3: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
     <t>They get an extra Star because their staff 8 of 10 have been polite. Drive through has issues. They constantly get order wrong. Ask you to pull forward to fix and leave you hanging. I have had to go in twice to see why I am still sitting after five minutes. They are new. I understand training new people. But when you place an order and they repeat it back correctly and it comes out wrong or you have to repeat 3 times to make sure they get it right. Someone inside needs to make sure they are reading the whole ticket. Not just a quarter pounder. Especially with the multi menu choice of adding bacon or lettuce and tomatoes. Their tea as of late has tasted like dish soap and their fountain drinks have a funky taste to them. Numerous times their fries have been under cooked.</t>
   </si>
   <si>
-    <t>{0: ['extra Star', 'staff'], 1: ['issues'], 2: ['order'], 3: [], 4: [], 5: [], 6: ['new people'], 7: ['order', 'times'], 8: ['inside needs', 'whole ticket'], 9: ['quarter pounder just'], 10: ['multi menu choice', 'bacon', 'lettuce', 'tomatoes'], 11: ['tea', 'dish soap', 'fountain drinks', 'taste'], 12: ['Numerous times', 'fries']}</t>
-  </si>
-  <si>
-    <t>{0: ['Star = extra', 'staff = polite'], 1: ['Drive = have'], 2: [], 3: [], 4: [], 5: [], 6: ['people = new'], 7: [], 8: ['ticket = whole'], 9: [], 10: ['menu = multi'], 11: ['tea = taste', 'taste = funky'], 12: ['times = numerous', 'fries = cooked']}</t>
+    <t>{0: ['staff'], 1: [], 2: ['order'], 3: [], 4: [], 5: [], 6: ['new people'], 7: ['order'], 8: [], 9: ['quarter pounder just'], 10: [], 11: [], 12: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('drive', 'have')], 2: [('staff', 'get')], 3: [('staff', 'hang')], 4: [('staff', 'have'), ('staff', 'sit')], 5: [], 6: [('staff', 'understand'), ('people', 'new')], 7: [('staff', 'place'), ('staff', 'repeat'), ('staff', 'come'), ('staff', 'have'), ('staff', 'get')], 8: [('staff', 'read')], 9: [], 10: [], 11: [], 12: [('time', 'numerous')]}</t>
   </si>
   <si>
     <t>Got Wrong orderÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½</t>
   </si>
   <si>
-    <t>{0: ['Wrong order']}</t>
-  </si>
-  <si>
-    <t>{0: ['order = wrong']}</t>
+    <t>{0: ['wrong order']}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'wrong')]}</t>
   </si>
   <si>
     <t>McDonald's is usually pretty bad about inventory shorts especially.
 The BBQ sauce, it's just a conspiracy but if you ever been a lover of Mcys Nuggets then you know they tend to "Forget" the BBQ sauce. Any other sauce and it's in there. But overall I dont see my self going back anytime soon.</t>
   </si>
   <si>
-    <t>{0: ['inventory shorts'], 1: ['conspiracy just', 'sauce'], 2: ['other sauce'], 3: ['self']}</t>
-  </si>
-  <si>
-    <t>{0: ['McDonald = bad'], 1: [], 2: ['sauce = other', "'s = other"], 3: ['self = go']}</t>
+    <t>{0: [], 1: ['conspiracy just', 'sauce'], 2: ['other sauce'], 3: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('mcdonald', 'know'), ('mcdonald', 'tend')], 2: [('sauce', 'other')], 3: [('mcdonald', 'see')]}</t>
   </si>
   <si>
     <t>So Uber eats was having connectivity issues and pushed an order through to this location that was supposed to be cancelled. I know this isnt McDonald's fault, but when I called McDonalds to try and address the issue, they answered and then ignored me and must have left their phone off the hook because any attempt to call them after this got me only dial tone. I know places are short staffed, but you cant just ignore people.</t>
   </si>
   <si>
-    <t>{0: ['connectivity issues', 'order'], 1: ['issue', 'phone', 'only dial tone only'], 2: ['places', 'people']}</t>
-  </si>
-  <si>
-    <t>{0: ['Uber = eat', 'eats = have'], 1: ['tone = only'], 2: []}</t>
+    <t>{0: ['order'], 1: ['issue'], 2: ['people']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [('place', 'ignore')]}</t>
   </si>
   <si>
     <t>If I paid for a large-sized meal, and I asked for both a large fry and a large drink, please don't argue with me that the ticket says medium drink. Thank you so much from a single parent who just wanted to spend a little bit of money on unhealthy food for wasting my hard-earned money.</t>
   </si>
   <si>
-    <t>{0: ['sized meal', 'large fry', 'large drink', 'ticket', 'medium drink'], 1: ['single parent', 'little bit', 'food', 'money']}</t>
-  </si>
-  <si>
-    <t>{0: ['meal = sized', 'drink = large', 'fry = large', 'drink = large', 'ticket = say', 'drink = medium'], 1: ['parent = single', 'bit = little', 'food = unhealthy']}</t>
+    <t>{0: ['large fry', 'large drink', 'medium drink'], 1: ['food', 'money']}</t>
+  </si>
+  <si>
+    <t>{0: [('fry', 'large'), ('drink', 'large'), ('drink', 'large'), ('drink', 'medium')], 1: [('food', 'unhealthy')]}</t>
   </si>
   <si>
     <t>Customer  service  is no good the staff  play games  as if I'm there to pay my money  to see them horsing around. And the the management  are a jock don't answer  the phone . to night is September 29 2021 at 10:30pm my next  visit to Austin will not be to a McDonald's...</t>
   </si>
   <si>
-    <t>{0: ['service', 'staff', 'games', 'money'], 1: ['management', 'phone'], 2: ['visit']}</t>
-  </si>
-  <si>
-    <t>{0: ['service = not good', 'staff = play'], 1: [], 2: ['visit = next']}</t>
+    <t>{0: ['service', 'staff'], 1: [], 2: ['visit']}</t>
+  </si>
+  <si>
+    <t>{0: [('staff', 'play'), ('service', 'horse')], 1: [], 2: [('visit', 'next')]}</t>
   </si>
   <si>
     <t>My nuggets were way to salty and crunchy which means to had been sitting there a while, cashier cut me off in the middle of my order but was nice and polite when I addressed it and fries where kinda cold but another then good place to get food at an affordable price</t>
   </si>
   <si>
-    <t>{0: ['nuggets', 'cashier', 'place', 'food', 'price']}</t>
-  </si>
-  <si>
-    <t>{0: ['cashier = cut', 'place = good', 'price = affordable']}</t>
+    <t>{0: ['place', 'food']}</t>
+  </si>
+  <si>
+    <t>{0: [('place', 'good')]}</t>
   </si>
   <si>
     <t>Alright I know it was 5:25 in the morning when we came here and the worker was probably tired as hell. I will give him that for sure, but it was just odd pulling up to the machine and total silence. we had to say "hello?" before he came on and asked what we wanted. Was seemingly rude about it and not amazingly friendly. You do not have to sound peppy and full of life at 5am, but at least be nice..</t>
   </si>
   <si>
-    <t>{0: ['worker'], 1: ['total silence'], 2: [], 3: [], 4: []}</t>
-  </si>
-  <si>
-    <t>{0: ['worker = tired'], 1: ['silence = total'], 2: [], 3: [], 4: []}</t>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: []}</t>
   </si>
   <si>
     <t>5 years ago</t>
@@ -757,16 +742,13 @@
     <t>waited in the drive through for over half an hour, all i got for my trouble was a "sorry for the wait" not even an explanation. When I got to the second window there were at least a dozen sodas just sitting on the counter. It's not the first time I've had bad service. I once pulled up and they just said we're not serving right now even though it was smack dab in the middle of the day hours.</t>
   </si>
   <si>
-    <t>{0: ['explanation even'], 1: ['second window', 'dozen least', 'dozen sodas'], 2: ['first time', 'service'], 3: ['dab smack', 'day hours']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['window = second'], 2: ['time = first', 'service = bad'], 3: []}</t>
+    <t>{0: ['explanation even'], 1: ['second window'], 2: ['first time', 'service'], 3: ['day hours']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('window', 'second')], 2: [('time', 'first'), ('service', 'bad')], 3: []}</t>
   </si>
   <si>
     <t>When you specifically say, ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½plain AND dryÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ and then just to make sure they understood (cuz letÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s face it, itÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s MacDonalds) you add - ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½so nothing but the meat and bunsÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½. Then you get home, open the bag, and immediately see the cheese through the hamburger wrapper.... I mean for cryin</t>
-  </si>
-  <si>
-    <t>{0: ['buns'], 1: ['bag', 'cheese', 'hamburger wrapper'], 2: []}</t>
   </si>
   <si>
     <t>{0: [], 1: [], 2: []}</t>
@@ -776,19 +758,19 @@
 Please be sure to check your order prior to leaving the premises. Do note that it takes forever to get them to correct their mistakes, so do take into consideration that the rest of your food will be cold and soggy by the time</t>
   </si>
   <si>
-    <t>{0: [], 1: ['food'], 2: ['particular location'], 3: ['location', 'items', 'order'], 4: ['order', 'premises'], 5: ['mistakes', 'rest']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['cheap = fast', 'food = fast'], 2: ['location = particular'], 3: ['location = love', 'items = incorrect', '% = incorrect', 'order = miss'], 4: [], 5: ['rest = cold', 'rest = soggy']}</t>
+    <t>{0: [], 1: ['food'], 2: ['particular location'], 3: ['location', 'order'], 4: ['order'], 5: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('food', 'fast')], 2: [('location', 'particular')], 3: [('location', 'love'), ('order', 'miss')], 4: [], 5: [('location', 'take'), ('location', 'correct')]}</t>
   </si>
   <si>
     <t>Service is slow, but I get all of my items with no errors and it's a bit smaller than most locations. Overall, it's a good place to grab a quick bite near Lake Creek.</t>
   </si>
   <si>
-    <t>{0: ['Service', 'most locations'], 1: ['place', 'quick bite']}</t>
-  </si>
-  <si>
-    <t>{0: ['Service = slow', 'locations = most'], 1: ['place = good', 'bite = quick']}</t>
+    <t>{0: ['service'], 1: ['place', 'quick bite']}</t>
+  </si>
+  <si>
+    <t>{0: [('service', 'get'), ('location', 'most')], 1: [('place', 'good'), ('bite', 'quick')]}</t>
   </si>
   <si>
     <t>The cashier's are very nice. Its very clean on the inside, and they get your food done fast</t>
@@ -797,16 +779,16 @@
     <t>{0: ['cashier'], 1: ['food']}</t>
   </si>
   <si>
-    <t>{0: ['cashier = nice'], 1: ['food = do']}</t>
+    <t>{0: [], 1: [('cashier', 'get'), ('food', 'do')]}</t>
   </si>
   <si>
     <t>Manager waited on me. He went out of his way to make me a satisfied customer.  Great customer service!</t>
   </si>
   <si>
-    <t>{0: [], 1: ['customer'], 2: ['Great customer service']}</t>
-  </si>
-  <si>
-    <t>{0: ['Manager = wait'], 1: ['customer = satisfied'], 2: ['service = great']}</t>
+    <t>{0: [], 1: ['customer'], 2: ['great customer service']}</t>
+  </si>
+  <si>
+    <t>{0: [('manager', 'wait')], 1: [('manager', 'go'), ('customer', 'satisfied')], 2: [('service', 'great')]}</t>
   </si>
   <si>
     <t>2:42 AM on a Saturday and they just straight up stopped answering the drive through. They just sitting in there chilling</t>
@@ -818,37 +800,37 @@
     <t>I would have given 5 stars, the evening manager is the nicest person I have seen and is definitely in charge of training her crew with constantly new help, in spite of this, everytime I have to return an order she goes back to the kitchen and patiently disassembles the sandwich and explains the proper way to make the sandwich in a spirit of education and with a cherry disposition. You can tell the children she works with respect her and look up to her, and yes, they might get things confused occasionally but I will continue to go there. 4 out of 5 stars</t>
   </si>
   <si>
-    <t>{0: ['stars', 'evening manager', 'person', 'crew', 'new help', 'order', 'sandwich', 'way', 'sandwich', 'cherry disposition'], 1: ['children', 'things'], 2: []}</t>
-  </si>
-  <si>
-    <t>{0: ['person = nice', 'help = new', 'way = proper'], 1: ['things = confuse'], 2: []}</t>
+    <t>{0: ['evening manager', 'order'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('manager', 'see'), ('manager', 'have'), ('manager', 'go')], 1: [('manager', 'tell'), ('manager', 'work'), ('manager', 'get')], 2: []}</t>
   </si>
   <si>
     <t>The staff is very kind and the food is usually prepared in a timely manner, for this reason it'sone of my preferred location's. However the drive thru line can sometimes be an inconvenience as it can get very long and at times even block entrances.</t>
   </si>
   <si>
-    <t>{0: ['staff', 'manner', 'preferred location'], 1: ['line', 'entrances']}</t>
-  </si>
-  <si>
-    <t>{0: ['staff = kind', 'manner = timely', 'location = preferred'], 1: []}</t>
+    <t>{0: ['staff', 'manner', 'preferred location'], 1: ['line']}</t>
+  </si>
+  <si>
+    <t>{0: [('manner', 'timely'), ('location', 'preferred')], 1: [('line', 'get')]}</t>
   </si>
   <si>
     <t>Awful experience. Drive thru attendants are rude, untrained, and unprofessional. When asked for a manager the attendants lie and say that there isn't one on duty, FYI impossible for every shift not to have a manager. One specific attendant screamed and cursed at me, to which led me to contact corporate.</t>
   </si>
   <si>
-    <t>{0: ['Awful experience'], 1: ['thru attendants'], 2: ['attendants', 'FYI', 'manager'], 3: ['specific attendant']}</t>
-  </si>
-  <si>
-    <t>{0: ['experience = awful'], 1: ['attendants = rude', 'attendants = untrained', 'attendants = unprofessional'], 2: ['attendants = lie'], 3: ['attendant = specific', 'attendant = scream']}</t>
+    <t>{0: ['awful experience'], 1: ['thru attendants'], 2: ['manager'], 3: ['specific attendant']}</t>
+  </si>
+  <si>
+    <t>{0: [('experience', 'awful')], 1: [], 2: [('attendant', 'lie')], 3: [('attendant', 'specific'), ('attendant', 'scream')]}</t>
   </si>
   <si>
     <t>Decent McDonald's location.  The team here has always been friendly.  Drive thru can get pretty backed up during normal meal periods, so often it is better to go inside.  Make sure you go close to regular meal periods for fresher food vs the ones under the heat lamp for a while.    Store is always clean.</t>
   </si>
   <si>
-    <t>{0: [], 1: ['team here'], 2: ['Drive thru', 'normal meal periods'], 3: ['regular meal periods', 'food', 'heat lamp'], 4: []}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['team = friendly'], 2: ['Drive = get', 'periods = normal', 'get = better'], 3: ['periods = regular', 'food = fresher'], 4: ['Store = clean']}</t>
+    <t>{0: [], 1: ['team here'], 2: ['drive thru'], 3: ['food'], 4: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [('drive', 'get'), ('period', 'normal')], 3: [('drive', 'go'), ('period', 'regular'), ('food', 'fresher')], 4: []}</t>
   </si>
   <si>
     <t>Hashbrowns were fire today.
@@ -856,101 +838,101 @@
 Always get me to work on time with fast workers</t>
   </si>
   <si>
-    <t>{0: ['Hashbrowns', 'fire today', 'machine'], 1: ['workers']}</t>
-  </si>
-  <si>
-    <t>{0: ['machine = work'], 1: ['workers = fast']}</t>
+    <t>{0: ['fire today', 'machine'], 1: []}</t>
+  </si>
+  <si>
+    <t>{0: [('machine', 'work')], 1: [('hashbrown', 'work')]}</t>
   </si>
   <si>
     <t>When I order during the day, I have zero issues. They are listed as a 24 hour location, so they show up on Uber Eats late at night. Anytime I order after midnight, they will accept my order through UE and then sit around for an hour before cancelling it. I don't understand why you list yourselves as a 24 hour location if you cancel any orders after midnight. Other than that, this place has always given great service.</t>
   </si>
   <si>
-    <t>{0: ['issues'], 1: ['hour location'], 2: ['order'], 3: ['yourselves', 'hour location', 'orders'], 4: ['place', 'service']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: [], 2: [], 3: [], 4: ['place = give', 'service = great']}</t>
+    <t>{0: [], 1: ['hour location'], 2: ['order'], 3: ['hour location'], 4: ['place', 'service']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [('place', 'give'), ('service', 'great')]}</t>
   </si>
   <si>
     <t>I ordered 4 happy meals with plain cheeseburgers. All the burgers were wrong. Do you know what itÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s like to have four grandkids that canÃÂ¯ÃÂ¿</t>
   </si>
   <si>
-    <t>{0: ['meals', 'plain cheeseburgers'], 1: ['burgers'], 2: ['like', 'grandkids']}</t>
-  </si>
-  <si>
-    <t>{0: ['meals = happy', 'cheeseburgers = plain'], 1: ['burgers = wrong'], 2: ['like = have']}</t>
+    <t>{0: ['plain cheeseburgers'], 1: [], 2: ['like']}</t>
+  </si>
+  <si>
+    <t>{0: [('cheeseburger', 'plain')], 1: [], 2: [('burger', 'know'), ('like', 'have')]}</t>
   </si>
   <si>
     <t>McDonalds is NOT a fast food company anymore. They're just a food company now. Always a line wrapped around the building that never moves. When are robots going to replace the kitchen staff who hate their jobs?</t>
   </si>
   <si>
-    <t>{0: ['food company'], 1: ['food company just'], 2: ['line Always'], 3: ['robots', 'kitchen staff', 'jobs']}</t>
-  </si>
-  <si>
-    <t>{0: ['food = fast'], 1: [], 2: [], 3: ['robots = go']}</t>
+    <t>{0: ['food company'], 1: ['food company just'], 2: ['line always'], 3: ['kitchen staff']}</t>
+  </si>
+  <si>
+    <t>{0: [('food', 'fast')], 1: [], 2: [('mcdonalds', 'move')], 3: []}</t>
   </si>
   <si>
     <t>This McDonalds CONSTANTLY gets orders wrong. We have ordered at the window and over uber and EVERY SINGLE TIME we dont get a complete order. Today we went back to get our fry we had 3 chicken sandwiches and 2 fry not complicated at all. The manager gave us a new one but the girl at the oick up window shoved the bag in ny hands and when I tha ked her she made a rude face and turned away.</t>
   </si>
   <si>
-    <t>{0: ['CONSTANTLY', 'orders'], 1: ['SINGLE TIME', 'complete order'], 2: ['fry', 'chicken sandwiches', 'fry'], 3: ['manager', 'new one', 'girl', 'bag'], 4: ['face']}</t>
-  </si>
-  <si>
-    <t>{0: ['CONSTANTLY = get'], 1: ['TIME = single', 'order = complete'], 2: ['SINGLE = go', 'fry = complicate', 'sandwiches = complicate'], 3: ['manager = give', 'one = new', 'girl = shove'], 4: ['face = rude']}</t>
+    <t>{0: [], 1: ['single time', 'complete order'], 2: ['fry', 'fry'], 3: ['manager', 'new one'], 4: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('time', 'single'), ('order', 'complete')], 2: [('fry', 'complicate')], 3: [('manager', 'give'), ('one', 'new'), ('manager', 'tha')], 4: [('manager', 'make')]}</t>
   </si>
   <si>
     <t>Night time drive through team seem really unprofessional. I ordered a meal with an extra fry, but when I got to the food window, was only given the fry with the meal. I mentioned the extra fry and was told I only paid for 1 fry. I offered to pay the difference for the extra fry, but was told I needed to drive back around and order again. Seriously? That's the response? Will not be returning.</t>
   </si>
   <si>
-    <t>{0: ['Night time'], 1: ['meal', 'extra fry', 'food window', 'fry'], 2: ['extra fry'], 3: ['difference', 'extra fry'], 4: [], 5: [], 6: []}</t>
-  </si>
-  <si>
-    <t>{0: ['time = drive', 'drive = seem'], 1: ['time = order', 'fry = extra'], 2: ['fry = extra'], 3: ['fry = extra'], 4: [], 5: [], 6: []}</t>
+    <t>{0: ['night time'], 1: ['extra fry', 'food window', 'fry'], 2: ['extra fry'], 3: ['extra fry'], 4: [], 5: [], 6: []}</t>
+  </si>
+  <si>
+    <t>{0: [('time', 'drive'), ('drive', 'seem')], 1: [('time', 'order'), ('fry', 'extra'), ('time', 'get')], 2: [('time', 'mention'), ('fry', 'extra'), ('time', 'pay')], 3: [('time', 'offer'), ('fry', 'extra'), ('time', 'need')], 4: [], 5: [], 6: []}</t>
   </si>
   <si>
     <t>This is the 3rd time in a row that weÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ve been burned going through the drive threw. Each time they have messed up our order and youÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½d think by now that I would have learned my lesson, but I thought this would be quick and easy. NOPE! This location sucks. I tried calling the number in the receipt but no one answers. I know I canÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½</t>
   </si>
   <si>
-    <t>{0: ['3rd time'], 1: ['order', 'lesson'], 2: [], 3: ['location'], 4: ['number'], 5: []}</t>
-  </si>
-  <si>
-    <t>{0: ['time = 3rd'], 1: [], 2: [], 3: ['location = suck'], 4: ['one = answer'], 5: []}</t>
+    <t>{0: ['3rd time'], 1: ['order'], 2: [], 3: ['location'], 4: [], 5: []}</t>
+  </si>
+  <si>
+    <t>{0: [('time', '3rd')], 1: [], 2: [], 3: [('location', 'suck')], 4: [('location', 'try'), ('one', 'answer')], 5: [('location', 'know')]}</t>
   </si>
   <si>
     <t>Worst experience! All I asked for was a regular size coffee.I get to the window and was handed a small , I asked the woman if that was a regular to which she rudely said yes I questioned her again two more times then I asked her how many sizes of coffee they had she said small medium and large I asked her which one was the one I was holding and she said it's a small that's what we charged you for she said, and I told her I asked for a regular which would be a medium but I just drove off. Also asked for 3 splendas and 4 creamers on the side and received 3 regular sugars and 2 creamers. To top it off, coffee was full of coffee grounds to the point I was spitting them out. And as a little plus there was a piece of plastic! Never again!</t>
   </si>
   <si>
-    <t>{0: ['Worst experience'], 1: ['regular size coffee'], 2: ['woman', 'more times', 'many sizes', 'small medium'], 3: [], 4: [], 5: ['regular sugars', 'creamers'], 6: ['coffee', 'coffee grounds'], 7: [], 8: []}</t>
-  </si>
-  <si>
-    <t>{0: ['experience = bad'], 1: ['size = regular'], 2: ['times = more', 'sizes = many', 'large = small', 'medium = small'], 3: [], 4: [], 5: ['sugars = regular', 'creamers = regular'], 6: ['coffee = full'], 7: [], 8: []}</t>
+    <t>{0: ['worst experience'], 1: ['regular size coffee'], 2: [], 3: [], 4: [], 5: ['regular sugars'], 6: ['coffee', 'coffee grounds'], 7: [], 8: []}</t>
+  </si>
+  <si>
+    <t>{0: [('experience', 'bad')], 1: [], 2: [('time', 'more')], 3: [], 4: [], 5: [], 6: [('coffee', 'spit')], 7: [], 8: []}</t>
   </si>
   <si>
     <t>Attempted to go through the drive thru at 430 am. It said it was 24 hour, however no one seemed to be taking orders and I drove around twice just in case and tried again but still no answer. I saw one employee in the kitchen but couldn't get his attention.   Very bad business. If closed or delayed in opening then at least a sign that indicates that would have been nice.</t>
   </si>
   <si>
-    <t>{0: [], 1: ['one', 'orders', 'answer still'], 2: ['employee', 'attention'], 3: ['business'], 4: ['opening then', 'sign least']}</t>
-  </si>
-  <si>
-    <t>{0: [], 1: ['one = seem'], 2: [], 3: ['business = bad'], 4: ['sign = least']}</t>
+    <t>{0: [], 1: ['one'], 2: ['employee'], 3: [], 4: ['opening then']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('one', 'seem'), ('one', 'drive')], 2: [('one', 'see')], 3: [], 4: [('one', 'indicate')]}</t>
   </si>
   <si>
     <t>This place is okay. It has these kiosks where you order, take a number, and they bring the food to your table. I ordered a frozen lemonade, paid for it, then sat down. I was there for a bit before someone came and told me they were out. I got a regular drink instead but it was too much trouble to get a refund for the difference. I'm not sure I like this new way.</t>
   </si>
   <si>
-    <t>{0: ['place'], 1: ['kiosks', 'number', 'food'], 2: ['lemonade'], 3: [], 4: ['regular drink'], 5: ['much trouble', 'refund'], 6: ['new way']}</t>
-  </si>
-  <si>
-    <t>{0: ['place = okay'], 1: [], 2: ['lemonade = frozen'], 3: [], 4: ['drink = regular'], 5: ['trouble = much'], 6: ['way = new']}</t>
+    <t>{0: ['place'], 1: ['food'], 2: [], 3: [], 4: ['regular drink'], 5: [], 6: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('place', 'have'), ('place', 'order'), ('place', 'bring')], 2: [('place', 'order')], 3: [('place', 'come')], 4: [('place', 'get'), ('drink', 'regular')], 5: [], 6: [('place', 'like')]}</t>
   </si>
   <si>
     <t>My burger was completely raw in the middle and when I took the burger back in to get it remade the lady behind the counter treated me like I was some stuck up brat for not wanting to eat a raw burger.
 If I had the ability to give them a zero star rating I would. I WILL NEVER EAT HERE AGAIN!!!</t>
   </si>
   <si>
-    <t>{0: ['burger', 'burger', 'lady', 'raw burger'], 1: ['ability', 'star rating'], 2: []}</t>
-  </si>
-  <si>
-    <t>{0: ['burger = raw', 'brat = stuck', 'burger = raw'], 1: [], 2: []}</t>
+    <t>{0: ['burger', 'burger', 'raw burger'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('burger', 'take'), ('burger', 'remade'), ('burger', 'raw')], 1: [('burger', 'have')], 2: []}</t>
   </si>
   <si>
     <t>If I could give negative stars I would. This location is the absolute worst ever.  Every single time I go they f up my order! Then give attitude when they need to correct their mistakes.  I Try to give the benefit of the doubt everyone has off/bad days so I return thinking this time will be different, but it never is. They always suck. The staff is horrible. Corporate needs to send all their staff over to a week of training at chic-fil-A college to learn about work ethic, time management ,teamwork and basic manors.
@@ -958,53 +940,56 @@
 Moral of rant save your time and money and drive around the corner to chic-fil-a they got your</t>
   </si>
   <si>
-    <t>{0: ['stars'], 1: ['location'], 2: ['single time'], 3: ['attitude', 'mistakes'], 4: ['benefit', 'days'], 5: ['time'], 6: [], 7: ['staff'], 8: ['staff', 'work ethic', 'time management', 'teamwork', 'basic manors'], 9: ['fil', 'cars', 'drive thru', 'order', 'first time'], 10: ['mins', 'order'], 11: ['sense'], 12: ['time', 'money']}</t>
-  </si>
-  <si>
-    <t>{0: ['stars = negative'], 1: [], 2: ['time = single'], 3: [], 4: ['days = bad'], 5: ['time = different'], 6: [], 7: ['staff = horrible'], 8: ['manors = basic'], 9: ['fil = chic', 'fil = have', 'time = first'], 10: [], 11: ['sense = logical'], 12: ['Moral = save', 'fil = chic']}</t>
+    <t>{0: [], 1: ['location'], 2: ['single time'], 3: [], 4: [], 5: ['time'], 6: [], 7: ['staff'], 8: ['staff', 'work ethic', 'time management'], 9: ['fil', 'drive thru', 'order', 'first time'], 10: ['order'], 11: [], 12: ['time']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [('time', 'single'), ('location', 'go')], 3: [('location', 'need')], 4: [('location', 'try'), ('location', 'have'), ('day', 'bad')], 5: [('location', 'return')], 6: [('time', 'suck')], 7: [], 8: [], 9: [('fil', 'chic'), ('fil', 'have'), ('time', 'first')], 10: [('fil', 'take')], 11: [], 12: [('fil', 'chic'), ('fil', 'get')]}</t>
   </si>
   <si>
     <t>When ordering food the employees conveniently forgot to turn off their microphones and were talking mess about all the food we had ordered, this is very unprofessional and honestly uncalled for. When I asked for a receipt they said it was in the bad and it was convenient not in there. IÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ve trying to get ahold of management to speak ab</t>
   </si>
   <si>
-    <t>{0: ['food', 'employees', 'microphones', 'mess'], 1: [], 2: []}</t>
-  </si>
-  <si>
-    <t>{0: ['employees = forget'], 1: [], 2: []}</t>
+    <t>{0: ['food'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('employee', 'forget'), ('employee', 'order')], 1: [('employee', 'ask'), ('employee', 'say')], 2: [('employee', 'try')]}</t>
   </si>
   <si>
     <t>I donÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t usually review places but this location has ridiculously rude service and consistently gets the orders wrong. Even when not busy. If I were rude, IÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
   </si>
   <si>
-    <t>{0: ['places', 'location', 'service', 'orders'], 1: [], 2: []}</t>
-  </si>
-  <si>
-    <t>{0: ['location = have', 'service = rude'], 1: [], 2: []}</t>
+    <t>{0: ['location', 'service'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('location', 'have'), ('service', 'rude')], 1: [], 2: []}</t>
   </si>
   <si>
     <t>Allways has the best Fries and Ice cream in the world!</t>
   </si>
   <si>
-    <t>{0: ['Allways', 'cream']}</t>
-  </si>
-  <si>
-    <t>{0: ['Allways = have', 'cream = good']}</t>
+    <t>{0: ['cream']}</t>
+  </si>
+  <si>
+    <t>{0: [('allway', 'have'), ('cream', 'good')]}</t>
   </si>
   <si>
     <t>Mcdonalds is great but they really need to hire people who understand both english and spanish and not just spanish speakers trying to take english orders. The people are really nice but be smarter about who you put in the drive thru and lobby to take orders.</t>
   </si>
   <si>
-    <t>{0: ['people', 'spanish speakers', 'english orders'], 1: ['people', 'orders']}</t>
-  </si>
-  <si>
-    <t>{0: ['Mcdonalds = great', 'speakers = spanish', 'speakers = try', 'orders = english'], 1: ['people = nice']}</t>
+    <t>{0: ['people', 'spanish speakers', 'english orders'], 1: ['people']}</t>
+  </si>
+  <si>
+    <t>{0: [('mcdonalds', 'need'), ('mcdonalds', 'understand'), ('order', 'english')], 1: [('people', 'put')]}</t>
+  </si>
+  <si>
+    <t>emotion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1017,6 +1002,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1054,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1064,6 +1057,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1367,20 +1363,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="180" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="77" customWidth="1"/>
-    <col min="5" max="5" width="41.109375" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="87" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="35.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1399,8 +1398,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G1" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1420,7 +1422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1500,7 +1502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1520,7 +1522,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1540,7 +1542,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1560,7 +1562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1680,7 +1682,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1720,7 +1722,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1740,7 +1742,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1760,7 +1762,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1800,7 +1802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1820,7 +1822,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="288" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1860,7 +1862,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1980,7 +1982,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2080,7 +2082,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2097,10 +2099,10 @@
         <v>123</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2108,19 +2110,19 @@
         <v>32</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2128,16 +2130,16 @@
         <v>68</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2148,19 +2150,19 @@
         <v>90</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D39">
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2168,19 +2170,19 @@
         <v>6</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D40">
         <v>5</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2188,39 +2190,39 @@
         <v>112</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2228,19 +2230,19 @@
         <v>32</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2248,16 +2250,16 @@
         <v>32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D44">
         <v>3</v>
       </c>
       <c r="E44" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2268,16 +2270,16 @@
         <v>68</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D45">
         <v>5</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2288,19 +2290,19 @@
         <v>90</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="F46" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2308,16 +2310,16 @@
         <v>32</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2328,19 +2330,19 @@
         <v>55</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2348,19 +2350,19 @@
         <v>32</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2368,19 +2370,19 @@
         <v>32</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2388,19 +2390,19 @@
         <v>32</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2408,19 +2410,19 @@
         <v>75</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2428,16 +2430,16 @@
         <v>32</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2448,19 +2450,19 @@
         <v>32</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2468,16 +2470,16 @@
         <v>32</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D55">
         <v>3</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2488,16 +2490,16 @@
         <v>68</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D56">
         <v>4</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -2508,7 +2510,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -2520,7 +2522,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2528,19 +2530,19 @@
         <v>32</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D58">
         <v>4</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2548,19 +2550,19 @@
         <v>32</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2568,19 +2570,19 @@
         <v>32</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D60">
         <v>4</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2588,19 +2590,19 @@
         <v>90</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2608,19 +2610,19 @@
         <v>75</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2628,16 +2630,16 @@
         <v>68</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>203</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -2648,19 +2650,19 @@
         <v>109</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2668,16 +2670,16 @@
         <v>32</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D65">
         <v>5</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2688,19 +2690,19 @@
         <v>109</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2708,16 +2710,16 @@
         <v>105</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2728,19 +2730,19 @@
         <v>90</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2748,19 +2750,19 @@
         <v>32</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D69">
         <v>2</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2768,19 +2770,19 @@
         <v>32</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2788,19 +2790,19 @@
         <v>32</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2808,16 +2810,16 @@
         <v>32</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2828,16 +2830,16 @@
         <v>32</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D73">
         <v>3</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -2848,36 +2850,36 @@
         <v>109</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D74">
         <v>3</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -2888,19 +2890,19 @@
         <v>109</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2908,19 +2910,19 @@
         <v>109</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2928,16 +2930,16 @@
         <v>32</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D78">
         <v>4</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2948,19 +2950,19 @@
         <v>32</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D79">
         <v>5</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2968,16 +2970,16 @@
         <v>32</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D80">
         <v>4</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2988,19 +2990,19 @@
         <v>68</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3008,16 +3010,16 @@
         <v>105</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D82">
         <v>4</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3028,19 +3030,19 @@
         <v>109</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D83">
         <v>4</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3048,36 +3050,36 @@
         <v>109</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D85">
         <v>3</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3088,19 +3090,19 @@
         <v>32</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D86">
         <v>5</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3108,19 +3110,19 @@
         <v>105</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D87">
         <v>3</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3128,19 +3130,19 @@
         <v>109</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3148,19 +3150,19 @@
         <v>32</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3168,16 +3170,16 @@
         <v>105</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3188,39 +3190,39 @@
         <v>32</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3228,39 +3230,39 @@
         <v>105</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D94">
         <v>1</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3268,16 +3270,16 @@
         <v>79</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D95">
         <v>3</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3288,19 +3290,19 @@
         <v>105</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D96">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3308,19 +3310,19 @@
         <v>79</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3328,19 +3330,19 @@
         <v>109</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D98">
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3348,16 +3350,16 @@
         <v>105</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D99">
         <v>1</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3368,19 +3370,19 @@
         <v>45</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D100">
         <v>5</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3388,16 +3390,16 @@
         <v>32</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D101">
         <v>4</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ability extraction for passive sentence
</commit_message>
<xml_diff>
--- a/delete.xlsx
+++ b/delete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baha Tegar\Desktop\aspect-based-sentiment-analysis-demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC43C4B3-6BD7-43BF-AFB9-1F6CC5010B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D10E97-F334-413A-9ED8-498DCA485EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1365,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="180" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Fix bug active sentence rules
</commit_message>
<xml_diff>
--- a/delete.xlsx
+++ b/delete.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baha Tegar\Desktop\aspect-based-sentiment-analysis-demo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E784BD8-33C5-46C4-B832-FEFFBB48E46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08541F85-6C99-42F1-A04C-E629B3E2DAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="372">
   <si>
     <t>reviewer_id</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>aspect</t>
+  </si>
+  <si>
+    <t>ability_old</t>
   </si>
   <si>
     <t>ability</t>
@@ -50,6 +53,9 @@
     <t>{0: [], 1: ['normal transaction'], 2: ['substance'], 3: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('transaction', 'normal')], 2: [('substance', 'milky'), ('substance', 'clear')], 3: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
@@ -60,6 +66,9 @@
   </si>
   <si>
     <t>{0: [], 1: ['food', 'atmosphere'], 2: ['staff here'], 3: [], 4: ['experience', 'food places']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('food', 'go'), ('atmosphere', 'go')], 2: [('staff', 'make')], 3: [('staff', 'friendly'), ('staff', 'accommodate'), ('staff', 'smile')], 4: [('experience', 'pleasant'), ('food', 'fast'), ('place', 'many'), ('place', 'other')]}</t>
   </si>
   <si>
     <t>{0: [], 1: [('food', 'go'), ('atmosphere', 'go')], 2: [('staff', 'does make difference')], 3: [('staff', 'are friendly'), ('staff', 'are accommodating'), ('staff', 'are smiling')], 4: []}</t>
@@ -75,18 +84,24 @@
     <t>{0: ['mobile order'], 1: ['line'], 2: [], 3: [], 4: ['next day', 'manager']}</t>
   </si>
   <si>
+    <t>{0: [('order', 'mobile'), ('order', 'get')], 1: [('line', 'move')], 2: [], 3: [('line', 'say')], 4: [('day', 'next'), ('manager', 'tell'), ('manager', 'wasn')]}</t>
+  </si>
+  <si>
     <t>{0: [('order', 'got'), ('order', 'got to speaker'), ('order', 'checked')], 1: [], 2: [], 3: [], 4: [('manager', 'told me')]}</t>
   </si>
   <si>
     <t>a month ago</t>
   </si>
   <si>
-    <t>My mc. Crispy chicken sandwich was ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿Ã</t>
+    <t>My mc. Crispy chicken sandwich was ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ customer service was quick and p</t>
   </si>
   <si>
     <t>{0: [], 1: ['crispy chicken sandwich', 'customer service']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('sandwich', 'crispy'), ('service', 'quick')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('service', 'was quick')]}</t>
   </si>
   <si>
@@ -99,6 +114,9 @@
     <t>{0: ['order', 'large meal double filet', 'large fries'], 1: ['drive thru']}</t>
   </si>
   <si>
+    <t>{0: [('filet', 'double'), ('fry', 'large')], 1: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: []}</t>
   </si>
   <si>
@@ -111,6 +129,9 @@
     <t>{0: ['door dash', 'long line'], 1: ['door dash'], 2: []}</t>
   </si>
   <si>
+    <t>{0: [('line', 'long')], 1: [('dash', 'door')], 2: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: []}</t>
   </si>
   <si>
@@ -120,6 +141,9 @@
     <t>{0: ['customer service'], 1: ['simple order'], 2: ['regular hamburg'], 3: [], 4: [], 5: ['one'], 6: [], 7: ['front counter'], 8: [], 9: ['order'], 10: [], 11: ['regular hamburg'], 12: [], 13: ['experience']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('order', 'simple')], 2: [('hamburg', 'regular')], 3: [], 4: [], 5: [], 6: [], 7: [('counter', 'front')], 8: [], 9: [], 10: [], 11: [('hamburg', 'regular')], 12: [], 13: [('experience', 'horrible')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [], 6: [], 7: [], 8: [], 9: [], 10: [], 11: [], 12: [], 13: []}</t>
   </si>
   <si>
@@ -132,6 +156,9 @@
     <t>{0: ['large coffee', 'ice'], 1: ['cup'], 2: ['employee', 'large coffee', 'ice'], 3: ['full cup'], 4: ['ice'], 5: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [], 3: [('cup', 'full')], 4: [('ice', 'large'), ('ice', 'sweet')], 5: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: []}</t>
   </si>
   <si>
@@ -141,12 +168,18 @@
     <t>{0: [], 1: [], 2: ['piece nuggets'], 3: [], 4: ['time'], 5: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [('time', 'hard')], 5: []}</t>
+  </si>
+  <si>
     <t>I'm not really a huge fan of fast food, but I have 2 teenage daughter's who enjoy McDs. The staff here is always friendly and ALWAYS get their orders correct. By far one of the best McDs I have ever been to. I always enjoy and appreciate quality service from quality people... and you'll definitely find it here. At least from the evening crew. Haven't been here during the day. My girls joke that I go here so often to get them food, that the staff is going to end up knowing me and having their order ready to go. Lmao Great people and excellent service. ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
   </si>
   <si>
     <t>{0: ['food'], 1: ['staff here'], 2: ['mcds'], 3: ['quality service', 'quality people'], 4: [], 5: [], 6: ['staff', 'order'], 7: ['great people', 'service']}</t>
   </si>
   <si>
+    <t>{0: [('food', 'fast')], 1: [('staff', 'friendly')], 2: [('mcds', 'good')], 3: [], 4: [], 5: [], 6: [('staff', 'go')], 7: [('service', 'great'), ('people', 'great'), ('service', 'excellent')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('staff', 'is friendly')], 2: [], 3: [], 4: [], 5: [], 6: [('staff', 'is going')], 7: []}</t>
   </si>
   <si>
@@ -154,6 +187,9 @@
   </si>
   <si>
     <t>{0: ['worst mcdonald']}</t>
+  </si>
+  <si>
+    <t>{0: [('mcdonald', 'bad')]}</t>
   </si>
   <si>
     <t>{0: []}</t>
@@ -170,6 +206,9 @@
     <t>{0: [], 1: ['long drive thru'], 2: ['food items'], 3: ['food item'], 4: [], 5: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('drive', 'long')], 2: [], 3: [], 4: [], 5: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [('order', 'was supposed to have items'), ('order', 'was supposed to have drinks')], 3: [], 4: [], 5: []}</t>
   </si>
   <si>
@@ -179,6 +218,9 @@
     <t>{0: ['morning crew'], 1: ['night crew', 'different experience', 'long waits'], 2: ['time occurrence'], 3: ['staff'], 4: ['order', 'single time']}</t>
   </si>
   <si>
+    <t>{0: [('crew', 'seem')], 1: [('experience', 'whole'), ('experience', 'different'), ('wait', 'long')], 2: [('crew', 'not bad')], 3: [('staff', 'rude')], 4: [('staff', 'mistake'), ('time', 'single')]}</t>
+  </si>
+  <si>
     <t>{0: [('crew', 'seems')], 1: [('crew', 'is whole different experience'), ('crew', 'is lines')], 2: [('crew', 'was occurrence'), ('crew', 'is nightly problem')], 3: [('staff', 'is rude')], 4: [('staff', 'will mistake well'), ('staff', 'will serve')]}</t>
   </si>
   <si>
@@ -188,6 +230,9 @@
     <t>{0: ['full order'], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
+    <t>{0: [('order', 'full')], 1: [], 2: [], 3: []}</t>
+  </si>
+  <si>
     <t>5 months ago</t>
   </si>
   <si>
@@ -197,18 +242,27 @@
     <t>{0: ['food burger', 'part'], 1: ['drink cup lid'], 2: ['poor service girl', 'order']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('one', 'fatten')], 2: []}</t>
+  </si>
+  <si>
     <t>This was a dine in experience. The tables were all dirty &amp; we did not get our food after waiting 35 minutes. Chicken sandwich was burnt.</t>
   </si>
   <si>
     <t>{0: [], 1: ['food'], 2: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('table', 'dirty')], 2: []}</t>
+  </si>
+  <si>
     <t>The line wS extremely big and was moving very slowly, plus they were out of apple pies and strawberry cream pies, but they gave me substitute cinnabun, the staff was very apologetic for being slow &amp; they were out of pies, but it was middle of the night and they were extremely under-staffed.</t>
   </si>
   <si>
     <t>{0: ['line', 'staff']}</t>
   </si>
   <si>
+    <t>{0: [('line', 'move'), ('line', 'give'), ('staff', 'apologetic'), ('line', 'middle'), ('line', 'staff')]}</t>
+  </si>
+  <si>
     <t>{0: [('line', 'was moving slowly'), ('line', 'was were'), ('line', 'was gave'), ('line', 'gave cinnabun'), ('staff', 'was apologetic'), ('line', 'were staffed')]}</t>
   </si>
   <si>
@@ -218,6 +272,9 @@
     <t>{0: ['boy', 'drink'], 1: []}</t>
   </si>
   <si>
+    <t>{0: [('boy', 'attend'), ('boy', 'make'), ('boy', 'see'), ('drink', 'wrong'), ('boy', 'throw')], 1: []}</t>
+  </si>
+  <si>
     <t>{0: [('boy', 'made'), ('boy', 'threw'), ('boy', 'attended'), ('drink', 'was wrong')], 1: []}</t>
   </si>
   <si>
@@ -230,6 +287,9 @@
     <t>{0: [], 1: ['smoothie'], 2: [], 3: [], 4: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('smoothie', 'taste')], 2: [], 3: [], 4: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('smoothie', 'should not never taste'), ('smoothie', 'should not never taste like that')], 2: [], 3: [], 4: []}</t>
   </si>
   <si>
@@ -237,6 +297,9 @@
   </si>
   <si>
     <t>{0: ['staff', 'perpetual learning']}</t>
+  </si>
+  <si>
+    <t>{0: [('staff', 'seem'), ('staff', 'make'), ('learning', 'perpetual'), ('staff', 'lead')]}</t>
   </si>
   <si>
     <t>{0: [('staff', 'seems'), ('staff', 'is'), ('staff', 'makes'), ('staff', 'can also lead')]}</t>
@@ -254,6 +317,9 @@
     <t>{0: ['experience', 'order taker'], 1: ['drive thru', 'employee'], 2: ['order', 'order'], 3: [], 4: [], 5: [], 6: ['order', 'time either'], 7: [], 8: [], 9: [], 10: [], 11: [], 12: [], 13: [], 14: ['order'], 15: [], 16: [], 17: ['window', 'next window'], 18: [], 19: ['next window', 'food'], 20: [], 21: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('employee', 'ask')], 2: [('employee', 'keep')], 3: [], 4: [], 5: [], 6: [], 7: [], 8: [], 9: [], 10: [], 11: [], 12: [], 13: [], 14: [], 15: [], 16: [('time', 'several')], 17: [('window', 'next')], 18: [], 19: [], 20: [], 21: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('employee', 'directly asks')], 2: [], 3: [], 4: [], 5: [], 6: [], 7: [], 8: [], 9: [], 10: [], 11: [], 12: [], 13: [], 14: [], 15: [], 16: [], 17: [], 18: [], 19: [], 20: [], 21: []}</t>
   </si>
   <si>
@@ -266,6 +332,9 @@
     <t>{0: ['meh just'], 1: ['order'], 2: [], 3: ['service industry'], 4: [], 5: ['order'], 6: ['order'], 7: [], 8: ['order'], 9: ['minute drive home'], 10: [], 11: ['evening staff', 'morning staff'], 12: [], 13: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('order', 'correct')], 2: [], 3: [], 4: [], 5: [('order', 'correct')], 6: [('order', 'correct')], 7: [], 8: [('fry', 'large')], 9: [], 10: [], 11: [('staff', 'pleasant'), ('staff', 'leave'), ('staff', 'talk'), ('staff', 'understand')], 12: [], 13: [('staff', 'wrong')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [('order', 'is correct')], 6: [('order', 'was correct')], 7: [], 8: [('order', 'was large fries'), ('order', 'was nothing')], 9: [], 10: [], 11: [('staff', 'is pleasant'), ('staff', 'leaves lot'), ('staff', 'thinking'), ('staff', 'can talk negatively'), ('staff', 'can talk about people'), ('staff', 'can talk in open'), ('staff', 'understand perfectly')], 12: [], 13: [('staff', 'is wrong')]}</t>
   </si>
   <si>
@@ -275,6 +344,9 @@
     <t>{0: ['caffeine'], 1: ['staff thru', 'drink'], 2: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('staff', 'shove')], 2: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('staff', 'just shoved'), ('staff', 'just shoved in hands')], 2: []}</t>
   </si>
   <si>
@@ -287,6 +359,9 @@
     <t>{0: ['meal'], 1: ['minute wait'], 2: [], 3: [], 4: ['meal', 'donation box']}</t>
   </si>
   <si>
+    <t>{0: [('meal', 'bad')], 1: [('wait', 'cold'), ('fry', 'cold')], 2: [], 3: [], 4: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: []}</t>
   </si>
   <si>
@@ -305,16 +380,22 @@
     <t>{0: ['ice cream machines'], 1: ['ice cream']}</t>
   </si>
   <si>
+    <t>{0: [('mcdonalds', 'proud')], 1: [('mcdonalds', 'have')]}</t>
+  </si>
+  <si>
     <t>With all the new upgrades everything looks great and clean great staff</t>
   </si>
   <si>
     <t>{0: ['new upgrades', 'staff']}</t>
   </si>
   <si>
+    <t>{0: [('upgrade', 'new'), ('staff', 'great'), ('staff', 'great')]}</t>
+  </si>
+  <si>
     <t>{0: [('everything', 'looks')]}</t>
   </si>
   <si>
-    <t>DoesnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯Ã</t>
+    <t>DoesnÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿</t>
   </si>
   <si>
     <t>Yet another McDonald's with horrible service and lazy employees. I mean c'mon do they intentionally hire unqualified people???</t>
@@ -323,6 +404,9 @@
     <t>{0: ['mcdonald yet', 'service'], 1: ['people']}</t>
   </si>
   <si>
+    <t>{0: [('service', 'horrible'), ('employee', 'lazy')], 1: [('people', 'unqualified')]}</t>
+  </si>
+  <si>
     <t>3 years ago</t>
   </si>
   <si>
@@ -330,6 +414,9 @@
   </si>
   <si>
     <t>{0: ['last time'], 1: [], 2: ['plain sausage biscuit', 'double quarter pounder'], 3: []}</t>
+  </si>
+  <si>
+    <t>{0: [('time', 'last')], 1: [], 2: [('sausage', 'plain'), ('quarter', 'double')], 3: []}</t>
   </si>
   <si>
     <t>2 years ago</t>
@@ -353,6 +440,9 @@
     <t>{0: ['location'], 1: ['people', 'parking lot', 'dinner food'], 2: ['parking lot', 'order menu'], 3: []}</t>
   </si>
   <si>
+    <t>{0: [('location', 'wack')], 1: [('location', 'stop'), ('people', 'sit'), ('people', 'get')], 2: [('time', 'multiple'), ('people', 'do')], 3: [('mcdonald', 'show')]}</t>
+  </si>
+  <si>
     <t>{0: [('location', 'is wack')], 1: [('location', 'will literally stop'), ('location', 'will make'), ('people', 'sit'), ('people', 'sit in lot'), ('people', 'sit for minutes'), ('people', 'sit until a.m.'), ('people', 'do not get anymore')], 2: [('people', 'do')], 3: []}</t>
   </si>
   <si>
@@ -362,12 +452,18 @@
     <t>{0: ['price'], 1: ['extra pickles']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('pickle', 'extra')]}</t>
+  </si>
+  <si>
     <t>Just spent 10 minutes waiting at this McDonald's . According to Google they're open 24/7. Finally we pull up to the window to see if anyone was there, sure enough one employee seated in the lobby and another at the window. She told me they were closed. Whoever these two are they need to be replaced. Get it together McDonald's. You're a corporate power house and you have a reputation to keep. One of the most unprofessional experiences I've ever had with fast food. 0/10 would not recomend this location.</t>
   </si>
   <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: ['mcdonald'], 6: [], 7: ['food'], 8: ['location']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [], 6: [], 7: [('experience', 'unprofessional'), ('food', 'fast')], 8: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [], 6: [], 7: [], 8: []}</t>
   </si>
   <si>
@@ -377,6 +473,9 @@
     <t>{0: [], 1: ['service']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('service', 'fast'), ('service', 'with')]}</t>
+  </si>
+  <si>
     <t>{0: [('everything', 'was great')], 1: [('service', 'is fast'), ('service', 'is with')]}</t>
   </si>
   <si>
@@ -386,6 +485,9 @@
     <t>{0: ['location', 'store'], 1: ['store'], 2: [], 3: []}</t>
   </si>
   <si>
+    <t>{0: [('store', 'horrible')], 1: [], 2: [], 3: []}</t>
+  </si>
+  <si>
     <t>{0: [('location', 'is horrible store')], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
@@ -395,12 +497,18 @@
     <t>{0: ['3rd time']}</t>
   </si>
   <si>
+    <t>{0: [('time', '3rd')]}</t>
+  </si>
+  <si>
     <t>The staff are very friendly and they do their job perfectly</t>
   </si>
   <si>
     <t>{0: ['staff', 'job']}</t>
   </si>
   <si>
+    <t>{0: [('staff', 'friendly'), ('staff', 'do')]}</t>
+  </si>
+  <si>
     <t>{0: [('staff', 'are friendly'), ('staff', 'do perfectly')]}</t>
   </si>
   <si>
@@ -408,6 +516,9 @@
   </si>
   <si>
     <t>{0: ['awesome service'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('service', 'awesome')], 1: [], 2: []}</t>
   </si>
   <si>
     <t>Went through the drive through ordered a large fry and two chicken deluxe sandwiches
@@ -419,6 +530,9 @@
     <t>{0: ['large fry', 'deluxe sandwiches', 'pay window', 'read back', 'spicey chicken sandwiches', 'deluxe crispy chicken sandwich'], 1: ['second time', 'order', 'spicey chicken sandwich', 'deluxe crispy chicken']}</t>
   </si>
   <si>
+    <t>{0: [('fry', 'large'), ('sandwich', 'deluxe'), ('sandwich', 'spicey')], 1: [('deluxe', 'say'), ('deluxe', 'fix'), ('time', 'second')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('deluxe', 'said'), ('deluxe', 'would fix then')]}</t>
   </si>
   <si>
@@ -431,12 +545,18 @@
     <t>{0: ['few orders', 'normal menu']}</t>
   </si>
   <si>
+    <t>{0: [('order', 'few'), ('menu', 'normal')]}</t>
+  </si>
+  <si>
     <t>This is the WORST McDonald's EVER, I don't come here often because when I do my order is wrong EVERY TIME.  Today 2/25/22 1130am 1 the drive thru person could barely hear me and I was almost yelling 2 I get to the next window after paying and I'm asked what did you order?? I tell them at the end of me repeating my order I now have your entire staff looking CONFUSED AS HELL like I just dropped outta the sky now I'm being asked did I pay? Are you sure you ordered at the speaker? Now all of ya'll wear head sets except for the cooks the worst leadership I've ever seen</t>
   </si>
   <si>
     <t>{0: ['worst mcdonald', 'order'], 1: ['drive thru person', 'next window'], 2: [], 3: ['order', 'entire staff'], 4: [], 5: [], 6: []}</t>
   </si>
   <si>
+    <t>{0: [('mcdonald', 'bad')], 1: [('window', 'next')], 2: [], 3: [('staff', 'entire'), ('staff', 'look')], 4: [], 5: [], 6: [('staff', 'wear')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [('staff', 'looking')], 4: [], 5: [], 6: [('staff', 'now wear sets'), ('staff', 'now wear except worst leadership')]}</t>
   </si>
   <si>
@@ -446,6 +566,9 @@
     <t>{0: ['food', 'mobile order'], 1: ['food', 'deal']}</t>
   </si>
   <si>
+    <t>{0: [('girlfriend', 'come'), ('order', 'mobile')], 1: [('food', 'taste')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('food', 'tasted')]}</t>
   </si>
   <si>
@@ -455,6 +578,9 @@
     <t>{0: ['location', 'few years'], 1: ['- day', 'night', 'food']}</t>
   </si>
   <si>
+    <t>{0: [('year', 'few')], 1: [('food', 'hot'), ('food', 'fresh')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('food', 'is hot'), ('food', 'is fresh')]}</t>
   </si>
   <si>
@@ -464,6 +590,9 @@
     <t>{0: ['employee']}</t>
   </si>
   <si>
+    <t>{0: [('employee', 'rude')]}</t>
+  </si>
+  <si>
     <t>{0: [('employee', 'was rude')]}</t>
   </si>
   <si>
@@ -473,6 +602,9 @@
     <t>{0: ['large fry buy'], 1: [], 2: [], 3: [], 4: [], 5: ['experience'], 6: ['order order', 'experience']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [('experience', 'bad')], 6: [('experience', 'exceptional')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [], 5: [], 6: []}</t>
   </si>
   <si>
@@ -488,6 +620,9 @@
     <t>{0: [], 1: ['one', 'iles ever'], 2: ['day'], 3: ['shift manager guy', 'black guy'], 4: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [('day', 'great')], 3: [('one', 'wrong'), ('guy', 'tall'), ('guy', 'black')], 4: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [('one', "'s wrong")], 4: []}</t>
   </si>
   <si>
@@ -497,12 +632,18 @@
     <t>{0: ['horrible service worker', 'stank attitude', 'window mute'], 1: ['order'], 2: ['long hair', 'meal fries', 'extra fry']}</t>
   </si>
   <si>
+    <t>{0: [('attitude', 'stank')], 1: [], 2: [('meal', 'happy'), ('fry', 'extra')]}</t>
+  </si>
+  <si>
     <t>Normally this location does pretty good, but last night was absolutely ridiculous. I sat in the drive thru for almost an hour waiting to get my order taken, the line was wrapped almost TWICE around the building, and finally I gave up and tried driving up to the window to give them my order since i was next in line. When i got to the window, they told me they couldn't take it and I'd have to go back around. I told them I'd like to put in my order here since I've been waiting all this time, and they proceeded to still refuse and that it's my fault for waiting in the second lane that they claimed was closed and had a sign out. The second lane was open, and the "sign" they were talking about was a wet floor sign they had placed right next to the drive-thru menu. I told them the lane looked open from our side and they still proceeded to argue with me, and then slammed the drive thru window shut. I've never received such deplorable customer service in my life, and if any managers are reading this, I highly suggest firing the two workers from last night.</t>
   </si>
   <si>
     <t>{0: ['location', 'last night'], 1: ['order', 'order'], 2: [], 3: [], 4: ['order', 'second lane', 'sign'], 5: ['second lane', 'sign', 'wet floor sign', 'thru menu'], 6: ['lane', 'window shut'], 7: ['customer service', 'last night']}</t>
   </si>
   <si>
+    <t>{0: [('night', 'last'), ('night', 'ridiculous')], 1: [('order', 'take')], 2: [('order', 'tell'), ('order', 'take')], 3: [], 4: [('order', 'proceed'), ('lane', 'second'), ('order', 'claim'), ('order', 'close')], 5: [('lane', 'second'), ('lane', 'open'), ('lane', 'talk'), ('lane', 'place')], 6: [('lane', 'look'), ('lane', 'proceed')], 7: [('service', 'such'), ('service', 'deplorable'), ('manager', 'read'), ('night', 'last')]}</t>
+  </si>
+  <si>
     <t>{0: [('night', 'was ridiculous')], 1: [('order', 'taken'), ('line', 'was wrapped almost TWICE around building')], 2: [('order', 'told me'), ('order', 'could not take it')], 3: [], 4: [('order', 'proceeded'), ('order', "'s"), ('order', 'closed'), ('order', 'claimed'), ('order', 'had')], 5: [('lane', 'was open'), ('sign', 'was sign'), ('lane', 'were talking'), ('lane', 'had placed next')], 6: [('lane', 'looked'), ('lane', 'proceeded'), ('lane', 'slammed'), ('lane', 'still proceeded'), ('lane', 'slammed')], 7: []}</t>
   </si>
   <si>
@@ -512,30 +653,45 @@
     <t>{0: ['location tonight'], 1: [], 2: []}</t>
   </si>
   <si>
+    <t>{0: [('mcdonalds', 'forget'), ('mcdonalds', 'refuse')], 1: [], 2: []}</t>
+  </si>
+  <si>
     <t>Rude customer service, unprofessional attitude, overcooked food, no complimentary items for screwing up our orders. I don't understand how you can keep your job when there is so many negative reviews. I vow to never eat here again. I would rather eat a cold can of baked beans...</t>
   </si>
   <si>
     <t>{0: ['rude customer service', 'overcooked food'], 1: [], 2: [], 3: ['can']}</t>
   </si>
   <si>
+    <t>{0: [('service', 'rude'), ('food', 'rude'), ('food', 'unprofessional'), ('food', 'overcooked')], 1: [], 2: [], 3: [('can', 'cold')]}</t>
+  </si>
+  <si>
     <t>Representative was very rude and disrespectful,  refused fulfilling my order and simply hung up on me on the drive through window... never was I so disappointed at that location before. Manager pretended like nothing even happened.</t>
   </si>
   <si>
     <t>{0: ['order'], 1: [], 2: ['manager']}</t>
   </si>
   <si>
+    <t>{0: [('representative', 'rude'), ('representative', 'disrespectful')], 1: [], 2: [('manager', 'pretend')]}</t>
+  </si>
+  <si>
     <t>They got our order correct and didn't cut me off before I had finished ordering our food at the speaker. I could actually understand our order taker. I don't know if it really gets any better than that at a fast food place anymore.</t>
   </si>
   <si>
     <t>{0: ['order', 'food'], 1: ['order taker'], 2: ['food place']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [('order', 'get'), ('place', 'fast')]}</t>
+  </si>
+  <si>
     <t>Good quick drive through service.  Was a long line but went very quickly.</t>
   </si>
   <si>
     <t>{0: ['quick drive'], 1: ['long line']}</t>
   </si>
   <si>
+    <t>{0: [('drive', 'good'), ('drive', 'quick')], 1: [('line', 'long')]}</t>
+  </si>
+  <si>
     <t>Yup. ItÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½s McDona</t>
   </si>
   <si>
@@ -545,6 +701,9 @@
     <t>{0: [], 1: ['great staff'], 2: ['food'], 3: [], 4: ['def customer service'], 5: [], 6: ['good customer service guys'], 7: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('staff', 'great')], 2: [], 3: [], 4: [('service', 'most'), ('service', 'def'), ('service', 'well')], 5: [('service', 'love')], 6: [], 7: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [('service', 'is better')], 5: [('service', 'love it')], 6: [], 7: []}</t>
   </si>
   <si>
@@ -554,6 +713,9 @@
     <t>{0: ['food', 'late night', 'drive through'], 1: ['order', 'one'], 2: ['hour'], 3: ['food', 'one', 'long time'], 4: []}</t>
   </si>
   <si>
+    <t>{0: [('night', 'late')], 1: [('one', 'come')], 2: [('one', 'take'), ('one', 'not good')], 3: [('one', 'care'), ('time', 'long')], 4: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('one', 'came'), ('one', 'came with food')], 2: [('one', 'is not good')], 3: [('one', 'cared'), ('one', 'cared about driver')], 4: []}</t>
   </si>
   <si>
@@ -563,6 +725,9 @@
     <t>{0: ['darn time'], 1: ['place'], 2: ['people'], 3: [], 4: [], 5: []}</t>
   </si>
   <si>
+    <t>{0: [('time', 'darn')], 1: [('place', 'open')], 2: [('place', 'find'), ('people', 'work')], 3: [('people', 'shower')], 4: [], 5: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('place', 'is open')], 2: [('people', 'to work here')], 3: [('people', 'do shower'), ('people', 'do brush'), ('people', 'do change')], 4: [('people', 'are robots')], 5: []}</t>
   </si>
   <si>
@@ -570,6 +735,9 @@
   </si>
   <si>
     <t>{0: ['order', 'person', 'order']}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'wrong'), ('person', 'need')]}</t>
   </si>
   <si>
     <t>{0: [('order', 'was wrong'), ('person', 'needs')]}</t>
@@ -582,6 +750,9 @@
     <t>{0: ['manager'], 1: ['manager didnt'], 2: [], 3: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [], 3: [('need', 'good')]}</t>
+  </si>
+  <si>
     <t>{0: [('manager', 'IS RUDE')], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
@@ -594,6 +765,9 @@
     <t>{0: ['order'], 1: ['young lady thru', 'order'], 2: ['second window'], 3: ['little bit just', 'order', 'lady', 'first window'], 4: [], 5: ['2nd window', 'second window'], 6: [], 7: ['order'], 8: ['second lady', 'manager']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('lady', 'young'), ('lady', 'keep')], 2: [('window', 'second'), ('lady', 'break')], 3: [('window', 'first')], 4: [], 5: [('lady', 'dismiss'), ('window', '2nd'), ('window', 'second')], 6: [], 7: [], 8: [('lady', 'second'), ('manager', 'dismiss')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('lady', 'kept')], 2: [('lady', 'almost broke'), ('lady', 'almost broke with stuff')], 3: [], 4: [], 5: [('lady', 'just dismissed'), ('lady', 'just dismissed to 2nd window'), ('lady', 'not were')], 6: [], 7: [], 8: [('manager', 'dismissed'), ('manager', 'dismissed with condescending')]}</t>
   </si>
   <si>
@@ -603,6 +777,9 @@
     <t>{0: ['order'], 1: ['prices here', 'total welcome change']}</t>
   </si>
   <si>
+    <t>{0: [('employee', 'seem'), ('order', 'quick'), ('order', 'nice')], 1: [('location', 'other'), ('change', 'total')]}</t>
+  </si>
+  <si>
     <t>{0: [('order', "'re quick"), ('order', "'re nice")], 1: []}</t>
   </si>
   <si>
@@ -612,12 +789,18 @@
     <t>{0: ['fry containers'], 1: [], 2: [], 3: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [('fry', 'not great')], 3: []}</t>
+  </si>
+  <si>
     <t>They get an extra Star because their staff 8 of 10 have been polite. Drive through has issues. They constantly get order wrong. Ask you to pull forward to fix and leave you hanging. I have had to go in twice to see why I am still sitting after five minutes. They are new. I understand training new people. But when you place an order and they repeat it back correctly and it comes out wrong or you have to repeat 3 times to make sure they get it right. Someone inside needs to make sure they are reading the whole ticket. Not just a quarter pounder. Especially with the multi menu choice of adding bacon or lettuce and tomatoes. Their tea as of late has tasted like dish soap and their fountain drinks have a funky taste to them. Numerous times their fries have been under cooked.</t>
   </si>
   <si>
     <t>{0: ['staff'], 1: [], 2: ['order'], 3: [], 4: [], 5: [], 6: ['new people'], 7: ['order'], 8: [], 9: ['quarter pounder just'], 10: [], 11: [], 12: []}</t>
   </si>
   <si>
+    <t>{0: [('staff', 'polite')], 1: [('drive', 'have')], 2: [('staff', 'get')], 3: [], 4: [], 5: [('staff', 'new')], 6: [('people', 'new')], 7: [('staff', 'repeat'), ('staff', 'come'), ('staff', 'get')], 8: [('staff', 'read')], 9: [], 10: [], 11: [], 12: [('time', 'numerous'), ('fry', 'cook')]}</t>
+  </si>
+  <si>
     <t>{0: [('staff', 'been polite')], 1: [], 2: [('staff', 'constantly get')], 3: [], 4: [], 5: [('staff', 'are new')], 6: [], 7: [('staff', 'repeat back correctly'), ('staff', 'get')], 8: [('staff', 'are reading')], 9: [], 10: [], 11: [], 12: []}</t>
   </si>
   <si>
@@ -625,6 +808,9 @@
   </si>
   <si>
     <t>{0: ['wrong order']}</t>
+  </si>
+  <si>
+    <t>{0: [('order', 'wrong')]}</t>
   </si>
   <si>
     <t>McDonald's is usually pretty bad about inventory shorts especially.
@@ -634,6 +820,9 @@
     <t>{0: [], 1: ['conspiracy just', 'sauce'], 2: ['other sauce'], 3: []}</t>
   </si>
   <si>
+    <t>{0: [('mcdonald', 'bad')], 1: [('mcdonald', 'tend')], 2: [('sauce', 'other')], 3: []}</t>
+  </si>
+  <si>
     <t>So Uber eats was having connectivity issues and pushed an order through to this location that was supposed to be cancelled. I know this isnt McDonald's fault, but when I called McDonalds to try and address the issue, they answered and then ignored me and must have left their phone off the hook because any attempt to call them after this got me only dial tone. I know places are short staffed, but you cant just ignore people.</t>
   </si>
   <si>
@@ -646,12 +835,18 @@
     <t>{0: ['large fry', 'large drink', 'medium drink'], 1: ['food', 'money']}</t>
   </si>
   <si>
+    <t>{0: [('drink', 'large'), ('fry', 'large'), ('drink', 'large'), ('drink', 'medium')], 1: [('food', 'unhealthy')]}</t>
+  </si>
+  <si>
     <t>Customer  service  is no good the staff  play games  as if I'm there to pay my money  to see them horsing around. And the the management  are a jock don't answer  the phone . to night is September 29 2021 at 10:30pm my next  visit to Austin will not be to a McDonald's...</t>
   </si>
   <si>
     <t>{0: ['service', 'staff'], 1: [], 2: ['visit']}</t>
   </si>
   <si>
+    <t>{0: [('service', 'not good'), ('staff', 'play'), ('service', 'horse')], 1: [], 2: [('visit', 'next')]}</t>
+  </si>
+  <si>
     <t>{0: [('service', 'is good'), ('staff', 'play'), ('service', 'horsing around')], 1: [], 2: []}</t>
   </si>
   <si>
@@ -661,6 +856,9 @@
     <t>{0: ['place', 'food']}</t>
   </si>
   <si>
+    <t>{0: [('place', 'good')]}</t>
+  </si>
+  <si>
     <t>Alright I know it was 5:25 in the morning when we came here and the worker was probably tired as hell. I will give him that for sure, but it was just odd pulling up to the machine and total silence. we had to say "hello?" before he came on and asked what we wanted. Was seemingly rude about it and not amazingly friendly. You do not have to sound peppy and full of life at 5am, but at least be nice..</t>
   </si>
   <si>
@@ -671,6 +869,9 @@
   </si>
   <si>
     <t>{0: ['explanation even'], 1: ['second window'], 2: ['first time', 'service'], 3: ['day hours']}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [('window', 'second')], 2: [('time', 'first'), ('service', 'bad')], 3: []}</t>
   </si>
   <si>
     <t>{0: [('all', 'was sorry for wait')], 1: [], 2: [], 3: []}</t>
@@ -686,6 +887,9 @@
     <t>{0: [], 1: ['food'], 2: ['particular location'], 3: ['location', 'order'], 4: ['order'], 5: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('food', 'fast')], 2: [('location', 'particular')], 3: [('location', 'love'), ('order', 'miss')], 4: [], 5: [('location', 'take'), ('location', 'correct')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [('location', 'is place')], 3: [('order', 'will missing')], 4: [], 5: [('location', 'to correct mistakes')]}</t>
   </si>
   <si>
@@ -695,12 +899,18 @@
     <t>{0: ['service'], 1: ['place', 'quick bite']}</t>
   </si>
   <si>
+    <t>{0: [('service', 'slow'), ('service', 'small'), ('location', 'most')], 1: [('place', 'good'), ('bite', 'quick')]}</t>
+  </si>
+  <si>
     <t>The cashier's are very nice. Its very clean on the inside, and they get your food done fast</t>
   </si>
   <si>
     <t>{0: ['cashier'], 1: ['food']}</t>
   </si>
   <si>
+    <t>{0: [('cashier', 'nice')], 1: [('cashier', 'get'), ('food', 'do')]}</t>
+  </si>
+  <si>
     <t>{0: [('cashier', 'are nice')], 1: [('cashier', 'get'), ('food', 'done fast')]}</t>
   </si>
   <si>
@@ -710,6 +920,9 @@
     <t>{0: [], 1: ['customer'], 2: ['great customer service']}</t>
   </si>
   <si>
+    <t>{0: [('manager', 'wait')], 1: [('manager', 'go'), ('customer', 'satisfied')], 2: [('service', 'great')]}</t>
+  </si>
+  <si>
     <t>2:42 AM on a Saturday and they just straight up stopped answering the drive through. They just sitting in there chilling</t>
   </si>
   <si>
@@ -722,6 +935,9 @@
     <t>{0: ['evening manager', 'order'], 1: [], 2: []}</t>
   </si>
   <si>
+    <t>{0: [('manager', 'go')], 1: [('manager', 'work'), ('manager', 'get')], 2: []}</t>
+  </si>
+  <si>
     <t>{0: [('manager', 'is nicest person'), ('manager', 'goes back'), ('manager', 'disassembles')], 1: [('manager', 'works'), ('manager', 'works with respect'), ('manager', 'works with her'), ('manager', 'might get')], 2: []}</t>
   </si>
   <si>
@@ -731,6 +947,9 @@
     <t>{0: ['staff', 'manner', 'preferred location'], 1: ['line']}</t>
   </si>
   <si>
+    <t>{0: [('staff', 'kind'), ('manner', 'timely'), ('location', 'preferred')], 1: [('line', 'get')]}</t>
+  </si>
+  <si>
     <t>{0: [('staff', 'is kind'), ('food', 'is prepared in timely manner'), ('food', 'is prepared for reason')], 1: [('line', 'be inconvenience')]}</t>
   </si>
   <si>
@@ -740,6 +959,9 @@
     <t>{0: ['awful experience'], 1: ['thru attendants'], 2: ['manager'], 3: ['specific attendant']}</t>
   </si>
   <si>
+    <t>{0: [('experience', 'awful')], 1: [('attendant', 'rude'), ('attendant', 'untrained'), ('attendant', 'unprofessional')], 2: [('attendant', 'lie')], 3: [('attendant', 'specific'), ('attendant', 'scream')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [('attendant', 'screamed'), ('attendant', 'cursed')]}</t>
   </si>
   <si>
@@ -747,6 +969,9 @@
   </si>
   <si>
     <t>{0: [], 1: ['team here'], 2: ['drive thru'], 3: ['food'], 4: []}</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [], 2: [('drive', 'get'), ('period', 'normal'), ('drive', 'well')], 3: [('period', 'regular'), ('food', 'fresher')], 4: []}</t>
   </si>
   <si>
     <t>Hashbrowns were fire today.
@@ -757,6 +982,9 @@
     <t>{0: ['fire today', 'machine'], 1: []}</t>
   </si>
   <si>
+    <t>{0: [('machine', 'work')], 1: []}</t>
+  </si>
+  <si>
     <t>{0: [('machine', 'is always working')], 1: []}</t>
   </si>
   <si>
@@ -766,6 +994,9 @@
     <t>{0: [], 1: ['hour location'], 2: ['order'], 3: ['hour location'], 4: ['place', 'service']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [], 3: [], 4: [('place', 'give'), ('service', 'great')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [('place', 'has always given')]}</t>
   </si>
   <si>
@@ -775,6 +1006,9 @@
     <t>{0: ['plain cheeseburgers'], 1: [], 2: ['like']}</t>
   </si>
   <si>
+    <t>{0: [('cheeseburger', 'plain')], 1: [('burger', 'wrong')], 2: [('like', 'have')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [('like', 'have grandkids')]}</t>
   </si>
   <si>
@@ -784,12 +1018,18 @@
     <t>{0: ['food company'], 1: ['food company just'], 2: ['line always'], 3: ['kitchen staff']}</t>
   </si>
   <si>
+    <t>{0: [('food', 'fast')], 1: [], 2: [('mcdonalds', 'move')], 3: []}</t>
+  </si>
+  <si>
     <t>This McDonalds CONSTANTLY gets orders wrong. We have ordered at the window and over uber and EVERY SINGLE TIME we dont get a complete order. Today we went back to get our fry we had 3 chicken sandwiches and 2 fry not complicated at all. The manager gave us a new one but the girl at the oick up window shoved the bag in ny hands and when I tha ked her she made a rude face and turned away.</t>
   </si>
   <si>
     <t>{0: [], 1: ['single time', 'complete order'], 2: ['fry', 'fry'], 3: ['manager', 'new one'], 4: []}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('time', 'single'), ('order', 'complete')], 2: [('fry', 'complicate')], 3: [('manager', 'give'), ('one', 'new')], 4: [('manager', 'make')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [('fry', 'not complicated all')], 3: [('manager', 'gave new one'), ('manager', 'shoved'), ('manager', 'ked')], 4: [('manager', 'made'), ('manager', 'turned')]}</t>
   </si>
   <si>
@@ -799,6 +1039,9 @@
     <t>{0: ['night time'], 1: ['extra fry', 'food window', 'fry'], 2: ['extra fry'], 3: ['extra fry'], 4: [], 5: [], 6: []}</t>
   </si>
   <si>
+    <t>{0: [('time', 'drive'), ('drive', 'seem')], 1: [('fry', 'extra')], 2: [('fry', 'extra')], 3: [('fry', 'extra')], 4: [], 5: [], 6: []}</t>
+  </si>
+  <si>
     <t>{0: [('time', 'drive through team'), ('drive', 'seem')], 1: [], 2: [], 3: [], 4: [], 5: [('time', "'s response")], 6: []}</t>
   </si>
   <si>
@@ -808,6 +1051,9 @@
     <t>{0: ['3rd time'], 1: ['order'], 2: [], 3: ['location'], 4: [], 5: []}</t>
   </si>
   <si>
+    <t>{0: [('time', '3rd')], 1: [], 2: [], 3: [('location', 'suck')], 4: [('one', 'answer')], 5: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [], 4: [('one', 'answers')], 5: []}</t>
   </si>
   <si>
@@ -817,6 +1063,9 @@
     <t>{0: ['worst experience'], 1: ['regular size coffee'], 2: [], 3: [], 4: [], 5: ['regular sugars'], 6: ['coffee', 'coffee grounds'], 7: [], 8: []}</t>
   </si>
   <si>
+    <t>{0: [('experience', 'bad')], 1: [], 2: [('time', 'more')], 3: [], 4: [], 5: [], 6: [('coffee', 'full')], 7: [], 8: []}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [('one', 'was one')], 3: [], 4: [], 5: [], 6: [('coffee', 'was full of grounds')], 7: [], 8: []}</t>
   </si>
   <si>
@@ -826,6 +1075,9 @@
     <t>{0: [], 1: ['one'], 2: ['employee'], 3: [], 4: ['opening then']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [('one', 'seem')], 2: [], 3: [], 4: [('one', 'indicate'), ('one', 'nice')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [('one', 'however seemed')], 2: [], 3: [], 4: [('one', 'indicates'), ('one', 'been nice')]}</t>
   </si>
   <si>
@@ -833,6 +1085,9 @@
   </si>
   <si>
     <t>{0: ['place'], 1: ['food'], 2: [], 3: [], 4: ['regular drink'], 5: [], 6: []}</t>
+  </si>
+  <si>
+    <t>{0: [('place', 'okay')], 1: [('place', 'have'), ('place', 'bring')], 2: [], 3: [('place', 'come')], 4: [('drink', 'regular')], 5: [], 6: []}</t>
   </si>
   <si>
     <t>{0: [('place', 'is okay')], 1: [('place', 'bring food'), ('place', 'bring to table')], 2: [], 3: [('place', 'came')], 4: [], 5: [], 6: []}</t>
@@ -843,6 +1098,9 @@
   </si>
   <si>
     <t>{0: ['burger', 'burger', 'raw burger'], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t>{0: [('burger', 'raw'), ('burger', 'remade'), ('burger', 'raw')], 1: [], 2: []}</t>
   </si>
   <si>
     <t>{0: [('burger', 'was raw')], 1: [], 2: []}</t>
@@ -856,6 +1114,9 @@
     <t>{0: [], 1: ['location'], 2: ['single time'], 3: [], 4: [], 5: ['time'], 6: [], 7: ['staff'], 8: ['staff', 'work ethic', 'time management'], 9: ['fil', 'drive thru', 'order', 'first time'], 10: ['order'], 11: [], 12: ['time']}</t>
   </si>
   <si>
+    <t>{0: [], 1: [], 2: [('time', 'single')], 3: [('location', 'need')], 4: [('location', 'have'), ('day', 'bad')], 5: [('time', 'different')], 6: [('time', 'suck')], 7: [('staff', 'horrible')], 8: [], 9: [('fil', 'chic'), ('fil', 'have'), ('time', 'first')], 10: [('fil', 'take')], 11: [], 12: [('fil', 'chic'), ('fil', 'get')]}</t>
+  </si>
+  <si>
     <t>{0: [], 1: [], 2: [], 3: [('location', 'need')], 4: [], 5: [('time', 'be different')], 6: [], 7: [('staff', 'is horrible')], 8: [], 9: [('fil', 'have cars')], 10: [], 11: [], 12: [('fil', 'got')]}</t>
   </si>
   <si>
@@ -865,12 +1126,18 @@
     <t>{0: ['food'], 1: [], 2: []}</t>
   </si>
   <si>
+    <t>{0: [('employee', 'forget'), ('employee', 'unprofessional'), ('employee', 'uncalled')], 1: [('employee', 'say'), ('employee', 'convenient')], 2: []}</t>
+  </si>
+  <si>
     <t>I donÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½t usually review places but this location has ridiculously rude service and consistently gets the orders wrong. Even when not busy. If I were rude, IÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯ÃÂ¿ÃÂ½ÃÂ¯</t>
   </si>
   <si>
     <t>{0: ['location', 'service'], 1: [], 2: []}</t>
   </si>
   <si>
+    <t>{0: [('location', 'have'), ('service', 'rude')], 1: [], 2: []}</t>
+  </si>
+  <si>
     <t>{0: [('location', 'have rude service')], 1: [], 2: []}</t>
   </si>
   <si>
@@ -880,10 +1147,16 @@
     <t>{0: ['cream']}</t>
   </si>
   <si>
+    <t>{0: [('allway', 'have'), ('cream', 'good')]}</t>
+  </si>
+  <si>
     <t>Mcdonalds is great but they really need to hire people who understand both english and spanish and not just spanish speakers trying to take english orders. The people are really nice but be smarter about who you put in the drive thru and lobby to take orders.</t>
   </si>
   <si>
     <t>{0: ['people', 'spanish speakers', 'english orders'], 1: ['people']}</t>
+  </si>
+  <si>
+    <t>{0: [('mcdonalds', 'great'), ('mcdonalds', 'need'), ('mcdonalds', 'understand'), ('order', 'english')], 1: [('people', 'nice')]}</t>
   </si>
   <si>
     <t>{0: [], 1: [('people', 'are nice')]}</t>
@@ -1262,20 +1535,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="61" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="47.109375" customWidth="1"/>
-    <col min="5" max="5" width="46.21875" customWidth="1"/>
-    <col min="6" max="6" width="62.33203125" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" customWidth="1"/>
+    <col min="5" max="5" width="42.88671875" customWidth="1"/>
+    <col min="6" max="6" width="44.44140625" customWidth="1"/>
+    <col min="7" max="7" width="53.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,2008 +1568,2312 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="216" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3">
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2">
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D18" s="2">
         <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="345.6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="D28" s="2">
         <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="D33" s="2">
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="D37" s="2">
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="D38" s="2">
         <v>1</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="D39" s="2">
         <v>5</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="D40" s="2">
         <v>5</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="D44" s="2">
         <v>3</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="D45" s="2">
         <v>5</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="D46" s="2">
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="D47" s="2">
         <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="D48" s="2">
         <v>1</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="288" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
       <c r="D50" s="2">
         <v>1</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="288" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="D55" s="2">
         <v>3</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="D56" s="2">
         <v>4</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="D57" s="2">
         <v>3</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="D58" s="2">
         <v>4</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>170</v>
+        <v>223</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="D60" s="2">
         <v>4</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="D61" s="2">
         <v>4</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>179</v>
+        <v>235</v>
       </c>
       <c r="D62" s="2">
         <v>1</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>182</v>
+        <v>239</v>
       </c>
       <c r="D63" s="2">
         <v>1</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
+        <v>55</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D64" s="2">
+      <c r="B64" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D64" s="3">
         <v>2</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E64" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>186</v>
+        <v>244</v>
       </c>
       <c r="D65" s="2">
         <v>5</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>187</v>
+        <v>245</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
       <c r="D66" s="2">
         <v>3</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>191</v>
+        <v>251</v>
       </c>
       <c r="D67" s="2">
         <v>2</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>194</v>
+        <v>255</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>195</v>
+        <v>256</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>196</v>
+        <v>258</v>
       </c>
       <c r="D69" s="2">
         <v>2</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>197</v>
+        <v>259</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>198</v>
+        <v>261</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>199</v>
+        <v>262</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>200</v>
+        <v>263</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>201</v>
+        <v>264</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>202</v>
+        <v>266</v>
       </c>
       <c r="D72" s="2">
         <v>1</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>203</v>
+        <v>267</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>205</v>
+        <v>270</v>
       </c>
       <c r="D73" s="2">
         <v>3</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>206</v>
+        <v>271</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>207</v>
+        <v>273</v>
       </c>
       <c r="D74" s="2">
         <v>3</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>209</v>
+        <v>275</v>
       </c>
       <c r="D75" s="2">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>210</v>
+        <v>276</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>212</v>
+        <v>279</v>
       </c>
       <c r="D76" s="2">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>213</v>
+        <v>280</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>214</v>
+        <v>281</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>216</v>
+        <v>284</v>
       </c>
       <c r="D78" s="2">
         <v>4</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>217</v>
+        <v>285</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>218</v>
+        <v>287</v>
       </c>
       <c r="D79" s="2">
         <v>5</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>219</v>
+        <v>288</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>221</v>
+        <v>291</v>
       </c>
       <c r="D80" s="2">
         <v>4</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>222</v>
+        <v>292</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>223</v>
+        <v>294</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>224</v>
+        <v>295</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>225</v>
+        <v>296</v>
       </c>
       <c r="D82" s="2">
         <v>4</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>226</v>
+        <v>297</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>228</v>
+        <v>300</v>
       </c>
       <c r="D83" s="2">
         <v>4</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>229</v>
+        <v>301</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>231</v>
+        <v>304</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>232</v>
+        <v>305</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>234</v>
+        <v>308</v>
       </c>
       <c r="D85" s="2">
         <v>3</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>235</v>
+        <v>309</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
       <c r="D86" s="2">
         <v>5</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>237</v>
+        <v>312</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>239</v>
+        <v>315</v>
       </c>
       <c r="D87" s="2">
         <v>3</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>240</v>
+        <v>316</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>242</v>
+        <v>319</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>243</v>
+        <v>320</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>245</v>
+        <v>323</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>246</v>
+        <v>324</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>247</v>
+        <v>326</v>
       </c>
       <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>248</v>
+        <v>327</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>250</v>
+        <v>330</v>
       </c>
       <c r="D91" s="2">
         <v>1</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>251</v>
+        <v>331</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="316.8" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>253</v>
+        <v>334</v>
       </c>
       <c r="D92" s="2">
         <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>254</v>
+        <v>335</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
+        <v>336</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
         <v>92</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D93" s="2">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
+      <c r="B93" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D93" s="3">
+        <v>1</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
         <v>93</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="D94" s="2">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B94" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D94" s="3">
+        <v>1</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>262</v>
+        <v>346</v>
       </c>
       <c r="D95" s="2">
         <v>3</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>263</v>
+        <v>347</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>265</v>
+        <v>350</v>
       </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>266</v>
+        <v>351</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>268</v>
+        <v>354</v>
       </c>
       <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>269</v>
+        <v>355</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>271</v>
+        <v>358</v>
       </c>
       <c r="D98" s="2">
         <v>1</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>272</v>
+        <v>359</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>273</v>
+        <v>361</v>
       </c>
       <c r="D99" s="2">
         <v>1</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>274</v>
+        <v>362</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>276</v>
+        <v>365</v>
       </c>
       <c r="D100" s="2">
         <v>5</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>277</v>
+        <v>366</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>278</v>
+        <v>368</v>
       </c>
       <c r="D101" s="2">
         <v>4</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>279</v>
+        <v>369</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>280</v>
+        <v>370</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>